<commit_message>
Program se automaticky vypne po 5 minutách
</commit_message>
<xml_diff>
--- a/prodeje.xlsx
+++ b/prodeje.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java\scraper_2.0\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="216">
   <si>
     <t>Item</t>
   </si>
@@ -663,6 +663,27 @@
   </si>
   <si>
     <t>prodáno</t>
+  </si>
+  <si>
+    <t>Bmw 325tds</t>
+  </si>
+  <si>
+    <t>70 000 Kč</t>
+  </si>
+  <si>
+    <t>02.12 2024 18:09</t>
+  </si>
+  <si>
+    <t>Chrudim 537 01</t>
+  </si>
+  <si>
+    <t>Prodám bmw e36 touring 2,5tds. Najeto 260 xxx Kastle bez rzi. Neschnilá jde zvedat za všechny zvedací body. Samozřejmě kosmetika je. Stk jsem dělal před zimou. Takže na necelé 2 roky klid. Bílá kůže Palubní počítač Všechny okna v elektrice. Tažné zařízení Na autě jsem dělal repas vstřikova ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/624/181027624.jpg?t=1707408320</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181027624/bmw-325tds.php</t>
   </si>
 </sst>
 </file>
@@ -1044,7 +1065,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4AC74AD-538C-4782-8A8D-C4C0C7DD934D}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
@@ -1052,17 +1073,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="74.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="35.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="255.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="96.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="117" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="54.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="51.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="74.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="31.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="35.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="25.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="31.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="255.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="96.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="117.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="54.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="36" x14ac:dyDescent="0.55000000000000004">
@@ -2167,6 +2188,35 @@
         <v>207</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>209</v>
+      </c>
+      <c r="C39" t="s">
+        <v>210</v>
+      </c>
+      <c r="D39" t="s">
+        <v>129</v>
+      </c>
+      <c r="E39" t="s">
+        <v>211</v>
+      </c>
+      <c r="F39" t="s">
+        <v>212</v>
+      </c>
+      <c r="G39" t="s">
+        <v>213</v>
+      </c>
+      <c r="H39" t="s">
+        <v>214</v>
+      </c>
+      <c r="I39" t="s">
+        <v>215</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Přidání ceny do finální tabulky
</commit_message>
<xml_diff>
--- a/prodeje.xlsx
+++ b/prodeje.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="345">
   <si>
     <t>Item</t>
   </si>
@@ -684,6 +684,393 @@
   </si>
   <si>
     <t>https://auto.bazos.cz/inzerat/181027624/bmw-325tds.php</t>
+  </si>
+  <si>
+    <t>bmw e46 323i</t>
+  </si>
+  <si>
+    <t>BMW E46</t>
+  </si>
+  <si>
+    <t>BMW E46, 323i(170koní), r.v.1999, 294tis.km, doklady DE</t>
+  </si>
+  <si>
+    <t>21.12. 2023</t>
+  </si>
+  <si>
+    <t>20.2. 2024</t>
+  </si>
+  <si>
+    <t>Příbram 262 42</t>
+  </si>
+  <si>
+    <t>Prodám spolehlivé coupe. Kosmetické vady, koroze blatníků, spodek zdravý, děravé není. Auto vlastním 4 roky, servis olejem samozřejmostí. Nové přední tlumiče, čelní okno, alternátor .Po technické stránce bezproblémové, motor v plné síle(M25B52), nehoupe, necvaká, nebere olej, voda čistá, neztrácí se ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/108/178806108.jpg?t=1703184999</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/178806108/bmw-e46-323i170koni-rv1999-294tiskm-doklady-de.php</t>
+  </si>
+  <si>
+    <t>bmw e39 523i</t>
+  </si>
+  <si>
+    <t>BMW E39</t>
+  </si>
+  <si>
+    <t>Bmw e39</t>
+  </si>
+  <si>
+    <t>16.2. 2024</t>
+  </si>
+  <si>
+    <t>Mělník 277 07</t>
+  </si>
+  <si>
+    <t>Prodám bmw e39 523i, rok 1998. nájezd 352xxxkm. Auto dovezeno z Itálie, naprosto bez známky koroze. motor m52b25. Auto vlastním cca rok a provedl jsem na něm velký servis: Nová spojka komplet přední náprava čidla abs silentbloky motoru silentbloky převodovky komplet čištění sání a škrtící klapky ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/985/181415985.jpg?t=1708185651</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181415985/bmw-e39.php</t>
+  </si>
+  <si>
+    <t>bmw e46 320d</t>
+  </si>
+  <si>
+    <t>BMW E46 320D 110Kw</t>
+  </si>
+  <si>
+    <t>18.2. 2024</t>
+  </si>
+  <si>
+    <t>Hodonín 696 72</t>
+  </si>
+  <si>
+    <t>Dobrý den BEZ KOROZE Motoricky TOP STAV nic nebouchá neklepe motor krásně tichý Plně pojízdné nikde mě nikdy nenechalo Vždy dostalo co potřebovalo Prodám bmw e46 320d 110Kw Velice zachovalé garážované bmw Nová STK do 15.1.2026 Nové přední destičky brembo Rok výroby 20.11.2003 Naj ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/607/181463607.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181463607/bmw-e46-320d-110kw.php</t>
+  </si>
+  <si>
+    <t>Bmw e46 320d 100kw</t>
+  </si>
+  <si>
+    <t>23.1. 2024</t>
+  </si>
+  <si>
+    <t>Vsetín 756 61</t>
+  </si>
+  <si>
+    <t>bmw e46 320d 100kw (jezdí bezproblému) Rok:27.7.2000 Naj:369114km 5.kvalt Stk:9/25 Vybava: 4x el.okna,klima (funkční)2din rádio android s parkovací kamerou,angel eyes (aliexpress)3 ramínko volant,latkové sedačky. Předchozí majitel dělal(muj známý) Silentbloky motoru Převodovky Diferenc ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/350/180254350.jpg?t=1708370328</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/180254350/bmw-e46-320d-100kw.php</t>
+  </si>
+  <si>
+    <t>bmw e46 330d</t>
+  </si>
+  <si>
+    <t>BMW E46 330D 135kw Automat xdrive 4x4</t>
+  </si>
+  <si>
+    <t>19.2. 2024</t>
+  </si>
+  <si>
+    <t>Cheb 352 01</t>
+  </si>
+  <si>
+    <t>Dobrý den, prodávám bmw e46 330d 135kw Automat, auto má najeto 292xxxkm co se týče auta jezdí hezky ,motor šlape jako hodinky, převodovka krásně řadí plynule bez škubání a podobně, na autě bylo dost investováno jako třeba snímač tlaků, kulový čep řízení levá pravá strana, manžeta kloubů,všechny filt ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/483/181555483.jpg?t=1708362859</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181555483/bmw-e46-330d-135kw-automat.php</t>
+  </si>
+  <si>
+    <t>Bmw E46 330D xdrive 135kw</t>
+  </si>
+  <si>
+    <t>25.1. 2024</t>
+  </si>
+  <si>
+    <t>Česká Lípa 471 56</t>
+  </si>
+  <si>
+    <t>Zdravím, mám tu na prodej bmw e46 330xd 135kw. Rok výroby 1999 Najeto 318 171 STK do 11/25 2din rádio s par. Kamerou Xenony Klimatizace Tempomat El.okna+zrcátka Dálkový centrál Čip na startování Palubní pc Mlhovky Kompletně černý interiér Síť v kufru pro psa Multifunkční volant DSC ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/893/180333893.jpg?t=1707115900</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/180333893/bmw-e46-330d-xdrive-135kw.php</t>
+  </si>
+  <si>
+    <t>Volkswagen Passat 1.9 tdi</t>
+  </si>
+  <si>
+    <t>Volkswagen Passat</t>
+  </si>
+  <si>
+    <t>VW Passat 1.9 TDI 96Kw, 4motion, nová Stk, serviska</t>
+  </si>
+  <si>
+    <t>Pelhřimov 394 61</t>
+  </si>
+  <si>
+    <t>volkswagen passat B5.5 1.9 tdi 4motion (4x4) 6q manuální převodovka Výroba: 12/2003 Nová Stk (do 02/2026) - 0 závad na protokolu Servisní kniha Nájezd: 246800 km Jsem druhý majitel vozu Nejvyšší výbava Highline Výbava: Tempomat, xenonové světlomety, multifunkční volant, vyhřívané sedačky, automa ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/341/181501341.jpg?t=1708286827</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181501341/vw-passat-19-tdi-96kw-4motion-nova-stk-serviska.php</t>
+  </si>
+  <si>
+    <t>Volkswagen Passat 1.9 TDI 96KW 6kavlt facelift R.V 2005</t>
+  </si>
+  <si>
+    <t>17.2. 2024</t>
+  </si>
+  <si>
+    <t>Pardubice 530 03</t>
+  </si>
+  <si>
+    <t>Prodám volkswagen passat 1.9 tdi 96KW 6 stupňová manuální převodovka Rok výroby 2005 Koupený V ČR Najeto 257 000 KM poctive 12 let jeden majitel Výbava El okna El zrcátka digitální klimatizace tempomat vyhřívaná sedadla palubní počítač 2x klíč a mnoha dalšího Vůz jezdí krásně a bez problémů a jeto ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/358/181447358.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181447358/volkswagen-passat-19-tdi-96kw-6kavlt-facelift-rv-2005.php</t>
+  </si>
+  <si>
+    <t>Volkswagen Passat //1.9TDi//96kW//6KVALT//2.MAJ//ČR//</t>
+  </si>
+  <si>
+    <t>15.2. 2024</t>
+  </si>
+  <si>
+    <t>Prostějov 796 01</t>
+  </si>
+  <si>
+    <t>R.V. 2002, NAJETO 259TKM SERVISNÍ KNÍŽKA. 2.MAJITEL KOUPENÉ JAKO NOVÉ V ČR. STK DO 2/2025. ---------------------------------------------------------------------- manuální převodovka 6 rychlostních stupňů přední pohon 4x airbag ABS stabilizace podvozku (ESP) senzor opotřebení brzdových dest ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/790/181354790.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181354790/volkswagen-passat-19tdi96kw6kvalt2majcr.php</t>
+  </si>
+  <si>
+    <t>Volkswagen Passat 2.0 tdi</t>
+  </si>
+  <si>
+    <t>Volkswagen Passat Variant 2.0TDi 103 kW, Aut. Klima</t>
+  </si>
+  <si>
+    <t>volkswagen passat Variant 2.0tdi, r.v. 2007, stav tachometru: 301694 Km, na voze pravidelný servis, STK do: 8/2024, 1968 CCM / 103 kW, VIN: WVWZZZ3CZ7E194678, Na všech vozech zajišťujeme i poprodejní servis, slušný stav vozu. MOŽNOST VYUŽITÍ FINANCOVÁNÍ VOZU JIŽ OD 10% AKONTACE !! Výbava: ABS, Orig ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/794/181544794.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181544794/volkswagen-passat-variant-20tdi-103-kw-aut-klima.php</t>
+  </si>
+  <si>
+    <t>Volkswagen passat b6 bez koroze</t>
+  </si>
+  <si>
+    <t>Prodam volkswagen passat b6 2.0tdi 103kw manual 6 kvalt rok vyroby 2007 najeto 280000km stk nova nic nehuči nic nemlati nova spojka komplet turbo Rozvody auto je bez zavad bez investice jen sednout a jezdit cena 59999kč dohoda možná</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/816/181543816.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181543816/volkswagen-passat-b6-bez-koroze.php</t>
+  </si>
+  <si>
+    <t>Prodám Volkswagen Passat B7, 2.0TDI 103kW</t>
+  </si>
+  <si>
+    <t>Chomutov 431 91</t>
+  </si>
+  <si>
+    <t>Prodám volkswagen passat B7, 2.0tdi 103kW, rok 2012 PROBLÉM S MOTOREM!! Motor dlouho točí, pak chytne, běží čistě a po chvíli chcipne jako kdyby došla nafta. Nehodlám dále řešit. Jinak vše funkční.</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/152/181367152.jpg?t=1708063979</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181367152/prodam-volkswagen-passat-b7-20tdi-103kw.php</t>
+  </si>
+  <si>
+    <t>Volkswagen Passat b5.5</t>
+  </si>
+  <si>
+    <t>Trutnov 543 01</t>
+  </si>
+  <si>
+    <t>2.0tdi 2005 290k km Po velkém servisu!! Více info po telefonu. Rozumná dohoda o ceně u auta!!</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/893/179103893.jpg?t=1707586062</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/179103893/volkswagen-passat-b55.php</t>
+  </si>
+  <si>
+    <t>Vw Passat B6 combi 2.0tdi 103kw</t>
+  </si>
+  <si>
+    <t>Nymburk 289 24</t>
+  </si>
+  <si>
+    <t>Prodám volkswagen passat B6 2.0tdi 103kw najeto 220.000km rok výroby 2007 v moc hezkém stavu absolutně bez koroze a v krásném laku. Auto bylo garážováno. Na autě proběhl servis olej v motoru včetně filtrů. Komplet rozvody ve 210.000km dále byla dělaná dvouhmota, nový alternator a nové brzdy. Auto má ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/998/178827998.jpg?t=1704633502</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/178827998/vw-passat-b6-combi-20tdi-103kw.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2 1.9 tdi</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2</t>
+  </si>
+  <si>
+    <t>8.2. 2024</t>
+  </si>
+  <si>
+    <t>Ústí nad Labem 400 07</t>
+  </si>
+  <si>
+    <t>1.9tdi 77kw r.v.2005,nová STK,xenony, vyhrev sedaček, climatronic, nyní po servisu olej+filtry, hydrosteli, rozvody,2x nové pneu Continental,hezký stav bez koroze, paket s vyšším podvozkem a plechovym krytem pod motorem, více info po tel.</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/982/181017982.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181017982/skoda-octavia-2.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2 1.9 TDI</t>
+  </si>
+  <si>
+    <t>7.2. 2024</t>
+  </si>
+  <si>
+    <t>Mělník 277 13</t>
+  </si>
+  <si>
+    <t>Prodám Škoda octavia 1.9tdi 77kw Najeto 434 000km Klimatizace Hansfree Zámek řazení Elektricky ovládané okna Elektricky ovládané zrcátka Čistý interiér Výškově nastavitelné sedačky Posilovač řízení Posilovač brzd Červená barva Stk do roku 2026</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/732/180980732.jpg?t=1707988891</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/180980732/skoda-octavia-2-19-tdi.php</t>
+  </si>
+  <si>
+    <t>Škoda octavia 2 1.9 tdi</t>
+  </si>
+  <si>
+    <t>6.2. 2024</t>
+  </si>
+  <si>
+    <t>Karviná 736 01</t>
+  </si>
+  <si>
+    <t>Vymenim Škoda octavia 2 1.9 tdi 77 kw. Rok vyrobí:2006 Najeto:284486 Stk:12/2025 Auto má vyhřívané sedačky. Auto je na celoročnich pneumatikach a přidám k tomu zimní pneu s disky Důvod prodeje, máme dva stejne auta a chtěl bych něco jineho takže nabidnete. Auto bez přepisu neodjede!</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/104/180927104.jpg?t=1707229184</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/180927104/skoda-octavia-2-19-tdi.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 1.9 tdi</t>
+  </si>
+  <si>
+    <t>Benešov 257 44</t>
+  </si>
+  <si>
+    <t>Prodám škodu Octavii II 1.9 tdi 77kw najeto 269000 rv 2008. Auto bez investic bez závad. Výbava tempomat, 4x El. okna, 2zonova klima, výhřev zrcátek, loketní opěrka, tažné zařízení, park. senzory. 2 klíče, zamykání zpatecky, zatmavena okna vzadu jako nova Jsem druhý majitel. Škoda octavia ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/366/180583366.jpg?t=1707137495</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/180583366/skoda-octavia.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2 1.9TDI 77kw BXE (ještě bez DPF)</t>
+  </si>
+  <si>
+    <t>14.1. 2024</t>
+  </si>
+  <si>
+    <t>Tábor 390 01</t>
+  </si>
+  <si>
+    <t>Dobrý den všem, prodám Octávii 2 77kw Combi Elegance 2006 335tKm, samotný motor šlape jak Švýcary jelikož už tam byl větší servis a láska po prvním majiteli, někdy ve 260tkm. Studené starty na brnknutí. TK 6/2024 Rozvody před 25tis, nový tlumič výfuku, nedávno dělané zavěšení ramen, zimní pneu 70 ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/222/179784222.jpg?t=1707716293</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/179784222/skoda-octavia-2-19tdi-77kw-bxe-jeste-bez-dpf.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2 2.0 tdi</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2.0 TDI. r.v.2015</t>
+  </si>
+  <si>
+    <t>Praha 4 147 00</t>
+  </si>
+  <si>
+    <t>Prodám octavia. 2.0,110kw,automatická převodovka DSG rok výroby 2015 po nehodě (foto).Při rychlém jednání možná sleva.</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/847/181344847.jpg?t=1707991214</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181344847/prodej.php</t>
+  </si>
+  <si>
+    <t>skoda fabia 1.4 mpi</t>
+  </si>
+  <si>
+    <t>skoda fabia</t>
+  </si>
+  <si>
+    <t>Koupím Škoda Fabia I - II 1.0 Mpi , 1.2 Mpi nebo 1.4 Mpi</t>
+  </si>
+  <si>
+    <t>Praha 10 109 00</t>
+  </si>
+  <si>
+    <t>Koupím ihned Škoda fabia I nebo II benzin , pouze zachovalou / ideálně originál stav /, dědictví , již nepotřebnou s rozumným nájezdem kilometrů a přiměřenou cenou dle stavu . Objem 1.0 nebo 1.2 Junior případně 1.4 . Nejsem bazar ani překupník . Cena do cca 30 tisíc u II dohodou . Nabídněte - ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/obrazky/empty.gif</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181544680/koupim-skoda-fabia-i-ii-10-mpi-12-mpi-nebo-14-mpi.php</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1452,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4AC74AD-538C-4782-8A8D-C4C0C7DD934D}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
@@ -2217,6 +2604,804 @@
         <v>215</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>216</v>
+      </c>
+      <c r="B40" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D40" t="s">
+        <v>217</v>
+      </c>
+      <c r="E40" t="s">
+        <v>218</v>
+      </c>
+      <c r="F40" t="n">
+        <v>61.0</v>
+      </c>
+      <c r="G40" t="s">
+        <v>219</v>
+      </c>
+      <c r="H40" t="s">
+        <v>220</v>
+      </c>
+      <c r="I40" t="s">
+        <v>221</v>
+      </c>
+      <c r="J40" t="s">
+        <v>222</v>
+      </c>
+      <c r="K40" t="s">
+        <v>223</v>
+      </c>
+      <c r="L40" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>225</v>
+      </c>
+      <c r="B41" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D41" t="s">
+        <v>226</v>
+      </c>
+      <c r="E41" t="s">
+        <v>227</v>
+      </c>
+      <c r="F41" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="G41" t="s">
+        <v>228</v>
+      </c>
+      <c r="H41" t="s">
+        <v>220</v>
+      </c>
+      <c r="I41" t="s">
+        <v>229</v>
+      </c>
+      <c r="J41" t="s">
+        <v>230</v>
+      </c>
+      <c r="K41" t="s">
+        <v>231</v>
+      </c>
+      <c r="L41" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>233</v>
+      </c>
+      <c r="B42" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>217</v>
+      </c>
+      <c r="E42" t="s">
+        <v>234</v>
+      </c>
+      <c r="F42" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G42" t="s">
+        <v>235</v>
+      </c>
+      <c r="H42" t="s">
+        <v>220</v>
+      </c>
+      <c r="I42" t="s">
+        <v>236</v>
+      </c>
+      <c r="J42" t="s">
+        <v>237</v>
+      </c>
+      <c r="K42" t="s">
+        <v>238</v>
+      </c>
+      <c r="L42" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>233</v>
+      </c>
+      <c r="B43" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>217</v>
+      </c>
+      <c r="E43" t="s">
+        <v>240</v>
+      </c>
+      <c r="F43" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="G43" t="s">
+        <v>241</v>
+      </c>
+      <c r="H43" t="s">
+        <v>220</v>
+      </c>
+      <c r="I43" t="s">
+        <v>242</v>
+      </c>
+      <c r="J43" t="s">
+        <v>243</v>
+      </c>
+      <c r="K43" t="s">
+        <v>244</v>
+      </c>
+      <c r="L43" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>246</v>
+      </c>
+      <c r="B44" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D44" t="s">
+        <v>217</v>
+      </c>
+      <c r="E44" t="s">
+        <v>247</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G44" t="s">
+        <v>248</v>
+      </c>
+      <c r="H44" t="s">
+        <v>220</v>
+      </c>
+      <c r="I44" t="s">
+        <v>249</v>
+      </c>
+      <c r="J44" t="s">
+        <v>250</v>
+      </c>
+      <c r="K44" t="s">
+        <v>251</v>
+      </c>
+      <c r="L44" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>246</v>
+      </c>
+      <c r="B45" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="C45" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D45" t="s">
+        <v>217</v>
+      </c>
+      <c r="E45" t="s">
+        <v>253</v>
+      </c>
+      <c r="F45" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="G45" t="s">
+        <v>254</v>
+      </c>
+      <c r="H45" t="s">
+        <v>220</v>
+      </c>
+      <c r="I45" t="s">
+        <v>255</v>
+      </c>
+      <c r="J45" t="s">
+        <v>256</v>
+      </c>
+      <c r="K45" t="s">
+        <v>257</v>
+      </c>
+      <c r="L45" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>259</v>
+      </c>
+      <c r="B46" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C46" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D46" t="s">
+        <v>260</v>
+      </c>
+      <c r="E46" t="s">
+        <v>261</v>
+      </c>
+      <c r="F46" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G46" t="s">
+        <v>248</v>
+      </c>
+      <c r="H46" t="s">
+        <v>220</v>
+      </c>
+      <c r="I46" t="s">
+        <v>262</v>
+      </c>
+      <c r="J46" t="s">
+        <v>263</v>
+      </c>
+      <c r="K46" t="s">
+        <v>264</v>
+      </c>
+      <c r="L46" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>259</v>
+      </c>
+      <c r="B47" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C47" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D47" t="s">
+        <v>260</v>
+      </c>
+      <c r="E47" t="s">
+        <v>266</v>
+      </c>
+      <c r="F47" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G47" t="s">
+        <v>267</v>
+      </c>
+      <c r="H47" t="s">
+        <v>220</v>
+      </c>
+      <c r="I47" t="s">
+        <v>268</v>
+      </c>
+      <c r="J47" t="s">
+        <v>269</v>
+      </c>
+      <c r="K47" t="s">
+        <v>270</v>
+      </c>
+      <c r="L47" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>259</v>
+      </c>
+      <c r="B48" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C48" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D48" t="s">
+        <v>260</v>
+      </c>
+      <c r="E48" t="s">
+        <v>272</v>
+      </c>
+      <c r="F48" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G48" t="s">
+        <v>273</v>
+      </c>
+      <c r="H48" t="s">
+        <v>220</v>
+      </c>
+      <c r="I48" t="s">
+        <v>274</v>
+      </c>
+      <c r="J48" t="s">
+        <v>275</v>
+      </c>
+      <c r="K48" t="s">
+        <v>276</v>
+      </c>
+      <c r="L48" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>278</v>
+      </c>
+      <c r="B49" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C49" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D49" t="s">
+        <v>260</v>
+      </c>
+      <c r="E49" t="s">
+        <v>279</v>
+      </c>
+      <c r="F49" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G49" t="s">
+        <v>248</v>
+      </c>
+      <c r="H49" t="s">
+        <v>220</v>
+      </c>
+      <c r="I49" t="s">
+        <v>114</v>
+      </c>
+      <c r="J49" t="s">
+        <v>280</v>
+      </c>
+      <c r="K49" t="s">
+        <v>281</v>
+      </c>
+      <c r="L49" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>278</v>
+      </c>
+      <c r="B50" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C50" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D50" t="s">
+        <v>260</v>
+      </c>
+      <c r="E50" t="s">
+        <v>283</v>
+      </c>
+      <c r="F50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G50" t="s">
+        <v>248</v>
+      </c>
+      <c r="H50" t="s">
+        <v>220</v>
+      </c>
+      <c r="I50" t="s">
+        <v>66</v>
+      </c>
+      <c r="J50" t="s">
+        <v>284</v>
+      </c>
+      <c r="K50" t="s">
+        <v>285</v>
+      </c>
+      <c r="L50" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>278</v>
+      </c>
+      <c r="B51" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C51" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D51" t="s">
+        <v>260</v>
+      </c>
+      <c r="E51" t="s">
+        <v>287</v>
+      </c>
+      <c r="F51" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G51" t="s">
+        <v>273</v>
+      </c>
+      <c r="H51" t="s">
+        <v>220</v>
+      </c>
+      <c r="I51" t="s">
+        <v>288</v>
+      </c>
+      <c r="J51" t="s">
+        <v>289</v>
+      </c>
+      <c r="K51" t="s">
+        <v>290</v>
+      </c>
+      <c r="L51" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>278</v>
+      </c>
+      <c r="B52" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C52" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D52" t="s">
+        <v>260</v>
+      </c>
+      <c r="E52" t="s">
+        <v>292</v>
+      </c>
+      <c r="F52" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="G52" t="s">
+        <v>254</v>
+      </c>
+      <c r="H52" t="s">
+        <v>220</v>
+      </c>
+      <c r="I52" t="s">
+        <v>293</v>
+      </c>
+      <c r="J52" t="s">
+        <v>294</v>
+      </c>
+      <c r="K52" t="s">
+        <v>295</v>
+      </c>
+      <c r="L52" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>278</v>
+      </c>
+      <c r="B53" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C53" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D53" t="s">
+        <v>260</v>
+      </c>
+      <c r="E53" t="s">
+        <v>297</v>
+      </c>
+      <c r="F53" t="n">
+        <v>61.0</v>
+      </c>
+      <c r="G53" t="s">
+        <v>219</v>
+      </c>
+      <c r="H53" t="s">
+        <v>220</v>
+      </c>
+      <c r="I53" t="s">
+        <v>298</v>
+      </c>
+      <c r="J53" t="s">
+        <v>299</v>
+      </c>
+      <c r="K53" t="s">
+        <v>300</v>
+      </c>
+      <c r="L53" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>302</v>
+      </c>
+      <c r="B54" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C54" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D54" t="s">
+        <v>191</v>
+      </c>
+      <c r="E54" t="s">
+        <v>303</v>
+      </c>
+      <c r="F54" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G54" t="s">
+        <v>304</v>
+      </c>
+      <c r="H54" t="s">
+        <v>220</v>
+      </c>
+      <c r="I54" t="s">
+        <v>305</v>
+      </c>
+      <c r="J54" t="s">
+        <v>306</v>
+      </c>
+      <c r="K54" t="s">
+        <v>307</v>
+      </c>
+      <c r="L54" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>302</v>
+      </c>
+      <c r="B55" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C55" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D55" t="s">
+        <v>191</v>
+      </c>
+      <c r="E55" t="s">
+        <v>309</v>
+      </c>
+      <c r="F55" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="G55" t="s">
+        <v>310</v>
+      </c>
+      <c r="H55" t="s">
+        <v>220</v>
+      </c>
+      <c r="I55" t="s">
+        <v>311</v>
+      </c>
+      <c r="J55" t="s">
+        <v>312</v>
+      </c>
+      <c r="K55" t="s">
+        <v>313</v>
+      </c>
+      <c r="L55" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>302</v>
+      </c>
+      <c r="B56" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C56" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D56" t="s">
+        <v>191</v>
+      </c>
+      <c r="E56" t="s">
+        <v>315</v>
+      </c>
+      <c r="F56" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="G56" t="s">
+        <v>316</v>
+      </c>
+      <c r="H56" t="s">
+        <v>220</v>
+      </c>
+      <c r="I56" t="s">
+        <v>317</v>
+      </c>
+      <c r="J56" t="s">
+        <v>318</v>
+      </c>
+      <c r="K56" t="s">
+        <v>319</v>
+      </c>
+      <c r="L56" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>302</v>
+      </c>
+      <c r="B57" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C57" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D57" t="s">
+        <v>191</v>
+      </c>
+      <c r="E57" t="s">
+        <v>321</v>
+      </c>
+      <c r="F57" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="G57" t="s">
+        <v>316</v>
+      </c>
+      <c r="H57" t="s">
+        <v>220</v>
+      </c>
+      <c r="I57" t="s">
+        <v>322</v>
+      </c>
+      <c r="J57" t="s">
+        <v>323</v>
+      </c>
+      <c r="K57" t="s">
+        <v>324</v>
+      </c>
+      <c r="L57" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>302</v>
+      </c>
+      <c r="B58" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C58" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D58" t="s">
+        <v>191</v>
+      </c>
+      <c r="E58" t="s">
+        <v>326</v>
+      </c>
+      <c r="F58" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="G58" t="s">
+        <v>327</v>
+      </c>
+      <c r="H58" t="s">
+        <v>220</v>
+      </c>
+      <c r="I58" t="s">
+        <v>328</v>
+      </c>
+      <c r="J58" t="s">
+        <v>329</v>
+      </c>
+      <c r="K58" t="s">
+        <v>330</v>
+      </c>
+      <c r="L58" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>332</v>
+      </c>
+      <c r="B59" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C59" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D59" t="s">
+        <v>191</v>
+      </c>
+      <c r="E59" t="s">
+        <v>333</v>
+      </c>
+      <c r="F59" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G59" t="s">
+        <v>273</v>
+      </c>
+      <c r="H59" t="s">
+        <v>220</v>
+      </c>
+      <c r="I59" t="s">
+        <v>334</v>
+      </c>
+      <c r="J59" t="s">
+        <v>335</v>
+      </c>
+      <c r="K59" t="s">
+        <v>336</v>
+      </c>
+      <c r="L59" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>338</v>
+      </c>
+      <c r="B60" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="C60" t="n">
+        <v>35000.0</v>
+      </c>
+      <c r="D60" t="s">
+        <v>339</v>
+      </c>
+      <c r="E60" t="s">
+        <v>340</v>
+      </c>
+      <c r="F60" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G60" t="s">
+        <v>248</v>
+      </c>
+      <c r="H60" t="s">
+        <v>220</v>
+      </c>
+      <c r="I60" t="s">
+        <v>341</v>
+      </c>
+      <c r="J60" t="s">
+        <v>342</v>
+      </c>
+      <c r="K60" t="s">
+        <v>343</v>
+      </c>
+      <c r="L60" t="s">
+        <v>344</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
úpravy ukládání topovaných inzerátů
</commit_message>
<xml_diff>
--- a/prodeje.xlsx
+++ b/prodeje.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="549">
   <si>
     <t>Item</t>
   </si>
@@ -1071,6 +1071,618 @@
   </si>
   <si>
     <t>https://auto.bazos.cz/inzerat/181544680/koupim-skoda-fabia-i-ii-10-mpi-12-mpi-nebo-14-mpi.php</t>
+  </si>
+  <si>
+    <t>BMW e46 320D, 110kw</t>
+  </si>
+  <si>
+    <t>27.1. 2024</t>
+  </si>
+  <si>
+    <t>21.2. 2024</t>
+  </si>
+  <si>
+    <t>Pardubice 530 09</t>
+  </si>
+  <si>
+    <t>Prodám bmw e46 320d, 110kw,6 rychlostí , Manuál ,rok výroby 2004, najeto 291tis výbava -el. okna, el. Zcratka , klimatizace , original rádio multifunkční volant , tempomat , automatické svícení, palubní počítač , kožená loketní opěrka atd atd Na autě jsou kosmetické vady, drobná koroze,original ...</t>
+  </si>
+  <si>
+    <t>https://cdn.discordapp.com/attachments/1063949035054051409/1209543945646768258/BMW_e46_320D_110kw.jpg?ex=65e74e94&amp;is=65d4d994&amp;hm=fe13ef8db2c994f25279c1037bacf1456f17fd5939d9786ea7bc57496058a237&amp;</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/180439669/bmw-e46-320d-110kw.php</t>
+  </si>
+  <si>
+    <t>bmw e46 320i</t>
+  </si>
+  <si>
+    <t>Koupim Bmw e46 320i drift</t>
+  </si>
+  <si>
+    <t>11.1. 2024</t>
+  </si>
+  <si>
+    <t>Trutnov 541 01</t>
+  </si>
+  <si>
+    <t>Koupim bmw e46 323i drift STK aspoň dva roky cena do 40000</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/179687874/koupim-bmw-e46-320i-drift.php</t>
+  </si>
+  <si>
+    <t>Bmw e46 323i coupe m-paket</t>
+  </si>
+  <si>
+    <t>Nový Jičín 742 35</t>
+  </si>
+  <si>
+    <t>Prodám bmw e46 323i coupe 125kw m52b25 R.v. 1999 Stk do 7/25 Dovoz z De v roce 2018 serviska vedena do 260tis. najeto 301xxxkm pruziny HaR, tlumice zadni bilstein,predni nove monroe, nove tycky stabiku,nove predni kotouce a desky Po výměně oleje+filtru ve 297xxxkm Baterie kupovaná 7/23 L ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/829/181401829.jpg?t=1708373224</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181401829/bmw-e46-323ci.php</t>
+  </si>
+  <si>
+    <t>BMW e39 523i</t>
+  </si>
+  <si>
+    <t>Hodonín 696 03</t>
+  </si>
+  <si>
+    <t>Prodám projekt na drift, jedná se o bmw e39 m52b25 vanos. Auto má zavařený diferenciál. Hydru- je potřeba zapojit. Bez zadních sedaček a interiéru , mám k autu. Bylo měněno těsnění pod hlavou. Platná STK a revize LPG, to ale není zapojeno. Více info tel. Dohoda možná.</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/673/181463673.jpg?t=1708401417</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181463673/bmw-e39-523i.php</t>
+  </si>
+  <si>
+    <t>BMW Řada 5, e39 523i 125kW.Automat.</t>
+  </si>
+  <si>
+    <t>12.2. 2024</t>
+  </si>
+  <si>
+    <t>Kutná Hora 284 01</t>
+  </si>
+  <si>
+    <t>bmw Řada 5, e39 523i 125kW.Automat. Najeto:317 247 km Vyrobeno:2/1999 VIN: WBADM41000GM05811 Specifikace vozu Karosérie:Sedan/limuzína Barva:Béžová Klimatizace:Automatická Počet airbagů:6 Počet dveří:5 Počet míst:5 Pohon Palivo:Benzín Objem:2 494 ccm Výkon:125 kW (170 koní) Převo ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/028/181228028.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181228028/bmw-rada-5-e39-523i-125kwautomat.php</t>
+  </si>
+  <si>
+    <t>BMW e46 320d 110kw</t>
+  </si>
+  <si>
+    <t>Ostrava 708 00</t>
+  </si>
+  <si>
+    <t>Prodám bmw e46 320d se spolehlivým dvou litrovým 110kw motorem. Datum výroby vozidla je 2002. Na autě žádná investice. Podvozek pevný. Motor suchý, čistý. Jen sednout a jezdit. Nájezd 310 XXX a km přibývají, s autem se jezdí. Dost věcí uděláno - turbo, všechny tlumiče, všechny žhavičky, spojka, celá ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/296/181314296.jpg?t=1708336512</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181314296/bmw-e46-320d-110kw.php</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/669/180439669.jpg?t=1707231766</t>
+  </si>
+  <si>
+    <t>BMW E46 330D 135kw Automat Xdrive 4x4</t>
+  </si>
+  <si>
+    <t>Dobrý den, prodávám bmw e46 330d 135kw Automat xdrive, auto má najeto 292xxxkm co se týče auta jezdí hezky ,motor šlape jako hodinky, převodovka krásně řadí plynule bez škubání a podobně, na autě bylo dost investováno jako třeba snímač tlaků, kulový čep řízení levá pravá strana, manžeta kloubů,všech ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/689/181592689.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181592689/bmw-e46-330d-135kw-automat-xdrive-4x4.php</t>
+  </si>
+  <si>
+    <t>Zdravím, mám tu na prodej bmw e46 330xd 135kw. Rok výroby 2000 Najeto 318 171 STK do 11/25 2din rádio s par. Kamerou Navigace Xenony Klimatizace Tempomat El.okna+zrcátka Dálkový centrál Čip na startování Palubní pc Mlhovky Zimní alu kola R17+ letní pneu k autu Kompletně černý interié ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/084/181581084.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181581084/bmw-e46-330d-xdrive-135kw.php</t>
+  </si>
+  <si>
+    <t>BMW E46 330d (135kw) M-Packet—Facelift-perleť 2003 ČÍST</t>
+  </si>
+  <si>
+    <t>Kolín 280 02</t>
+  </si>
+  <si>
+    <t>Prodam bmw e46 330d (135kw-Chip AC SCHNITZER 164kw jednotka) M-packet Combi/touring R.v. 2003 Stav tachometru: 380.000km (original) Motoricky v bezvadné kondici!!! Stk 10/2025 Cerny metalicky lak původní, po celolaku 2 roky zpět hnědá perleť. 1x klíček (nejde central) Nefunkční rucni bzda, ko ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/163/181407163.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181407163/bmw-e46-330d-135kw-m-packetfacelift-perlet-2003-cist.php</t>
+  </si>
+  <si>
+    <t>Volkswagen PASSAT B6</t>
+  </si>
+  <si>
+    <t>Ústí nad Labem 400 11</t>
+  </si>
+  <si>
+    <t>1.9tdi 77kw 375000km STK 05.25</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/471/181234471.jpg?t=1708030485</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181234471/volkswagen-passat-b6.php</t>
+  </si>
+  <si>
+    <t>Volkswagen Passat Kombi B 5.5 // 1.9 TDI 96kw // PĚKNÝ STAV</t>
+  </si>
+  <si>
+    <t>České Budějovice 370 01</t>
+  </si>
+  <si>
+    <t>PRODÁM: volkswagen passat Kombi B5,5 1.9 tdi - 96kw. Rok výroby 12/2003 v provozu od 1/2004. Již novější model FACELIFT!! Plní EURO 3. Přepis na nového majitele pouze 800kč. Vozidlo má všechny platné České doklady, evidenční kontrola platná, při koupi si přivezte ověřenou plnou moc, vozidlo na Vás p ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/048/181280048.jpg?t=1707852757</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181280048/volkswagen-passat-kombi-b-55-19-tdi-96kw-pekny-stav.php</t>
+  </si>
+  <si>
+    <t>Volkswagen passat 1.9 tdi 96KW</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/063/181604063.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181604063/volkswagen-passat-19-tdi-96kw.php</t>
+  </si>
+  <si>
+    <t>Volkswagen Passat 1.9TDI 77Kw Rezervace</t>
+  </si>
+  <si>
+    <t>R.v 2005, Najeto poctivých 285.000km, Dovoz z Německa, Po dohodě lze zařídit kompletní přihlášení, Nová stk 02/2026, Pravidelně servisováno, Rozvody při 281.000km Zimní kola, Tažné zařízení, Šíbr, Manuální 5 rychlostní převodovka Klimatizace, Isofix, Vyhřívaná sedadla, Vůz bez ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/691/181185691.jpg?t=1708325484</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181185691/volkswagen-passat-19tdi-77kw-comfort-tazne.php</t>
+  </si>
+  <si>
+    <t>VW Passat Variant 1.9 TDi, 81kw Automat, Itálie</t>
+  </si>
+  <si>
+    <t>22.12. 2023</t>
+  </si>
+  <si>
+    <t>Vsetín 755 01</t>
+  </si>
+  <si>
+    <t>Technické údaje _______________ Provoz od : 10/1998 Karosérie: combi, 5 dv., 5 míst Barva: šedá Obsah motoru: 1896cm Druh paliva: nafta Platnost STK do: 08/2025 Stav tachometru: 289 713 km Výkon motoru: 81kw __________________________ Cena: 41111kč nelze odečíst DPH _____________ ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/203/178867203.jpg?t=1707856437</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/178867203/volkswagen-passat-combi-19-tdi-81kw-automat-1majitel.php</t>
+  </si>
+  <si>
+    <t>Volkswagen Passat Variant 2.0TDI,Highline</t>
+  </si>
+  <si>
+    <t>Havlíčkův Brod 580 01</t>
+  </si>
+  <si>
+    <t>Prodám passat B6,2006 Bez DPF s platnou STK do 6.2015 je to manuál 6kvalt.Výbava Highline xenony všechny okna zrcátka v el.vcetně předních sedaček.Interiér pěkný nepotrhaný kůže+alcantara. Velká navigace s parkovacím kamerou.Na autě BBS 17R se zimní pneumatikou.Bude potřeba do budoucna udělat si o ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/349/181583349.jpg?t=1708418320</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181583349/volkswagen-passat-variant-20tdihighline.php</t>
+  </si>
+  <si>
+    <t>Volkswagen passat b6 variant 2.0tdi bez koroze</t>
+  </si>
+  <si>
+    <t>Prodam volkswagen passat b6 2.0tdi 103kw manual 6 kvalt rok vyroby 2007 najeto 280000km stk nova nic nehuči nic nemlati nova spojka komplet turbo Rozvody auto je bez zavad bez investice jen sednout a jezdit cena 63000kč dohoda možná</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/285/181578285.jpg?t=1708412682</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181578285/volkswagen-passat-b6-variant-20tdi-bez-koroze.php</t>
+  </si>
+  <si>
+    <t>Volkswagen Passat B6</t>
+  </si>
+  <si>
+    <t>Kroměříž 768 61</t>
+  </si>
+  <si>
+    <t>Prodám volkswagen passat B6 combi 2.0 tdi 103kw 6 st. Manuál rok výroby 2008 najeto poctivých 296xxxkm STK Platná Výbava: Highline 4x El.okna, El zrcátka, dvouzonová digitální klimatizace, palubní PC, tempomat, multifunkční volant, senzor deště, natáčecí xenony Angel eyes, parkovací senzory, záme ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/780/181535780.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181535780/volkswagen-passat-b6.php</t>
+  </si>
+  <si>
+    <t>Volkswagenu passat b6 2.0 tdi</t>
+  </si>
+  <si>
+    <t>Praha 8 182 00</t>
+  </si>
+  <si>
+    <t>Prodám volkswagen passat b6 rok 2007 2.0tdi 103kw , manuál 6q , stk 5/2025 Kožený sedačky s alcantarou ( nepotrhany ) elektricky - vyhrivany , tenpomat , aut. Světla , navi Couvaci kamera s asistentem ,senzory ,2din autorádio , automatická dvouzonova klima , a mnoho dalšího , Novy pneu , olej ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/481/181513481.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181513481/volkswagenu-passat-b6-20-tdi.php</t>
+  </si>
+  <si>
+    <t>Volkswagen Passat B6 2.0 TDI 103 KW FACELIFT</t>
+  </si>
+  <si>
+    <t>Kolín 281 01</t>
+  </si>
+  <si>
+    <t>volkswagen passat B6 2.0 tdi 103 Kw Sportline Common-Rail Najeto 284xxx STK 8/24 2x klíče R.V 2008 Typ motoru : CBAB 2x Vyhrivana sedadla tažné zařízení ( 1800 kg ) Podvozek pevný, tuhý bez vůli Výbava Sportline: Prisvit do zatacek,tažné zařízení, parkovací senzory, dotykove autorádio ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/364/181402364.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181402364/volkswagen-passat-b6-20-tdi-103-kw-facelift.php</t>
+  </si>
+  <si>
+    <t>VW Passat b6 2.0tdi dsg Zamluveno</t>
+  </si>
+  <si>
+    <t>Benešov 257 56</t>
+  </si>
+  <si>
+    <t>Prodam Pasika dsg r.v. 07 najeto 330tis. Automat,plna výbava,tažné nová STK . Stačí vaše plna moc auto prevedu. Prosím otázky jak mám dlouho proč prodavam atd. mi nedávejte děkuji. Auto každý den v provozu. Jako volkswagen Mercedes Skoda Bmw Kia Seat</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/085/181336085.jpg?t=1708407268</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181336085/vw-passat-b6-20tdi-dsg.php</t>
+  </si>
+  <si>
+    <t>Volkswagen Passat Variant 2.0TDi B6 103kw</t>
+  </si>
+  <si>
+    <t>14.2. 2024</t>
+  </si>
+  <si>
+    <t>Břeclav 691 52</t>
+  </si>
+  <si>
+    <t>Prodám volkswagen passat Variant Highline 2.0tdi B6 103kw, r.v. 2005,naj. 328 000km. Velmi dobrý optický i technický stav. Bez koroze a vždy garážované. Denně jezdí po dálnici, nevybydlené, nehavarované ,žádný tuning, vše v původním stavu. Včetně letních orig. 17 alu. Kilometry lze doložit, auto mám ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/620/181297620.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181297620/volkswagen-passat-variant-20tdi-b6-103kw.php</t>
+  </si>
+  <si>
+    <t>Volkswagen Passat B6 2.0TDI</t>
+  </si>
+  <si>
+    <t>13.2. 2024</t>
+  </si>
+  <si>
+    <t>Dobrý den, mám na prodej passat b6. 2007,BMP 103kw. Tachometr 239k kompletně vyměněn olej a filtr, nové brzdy, kompletně vyrobená pdvozku vozidla STK hotovo do roku 2026, pokud máte dotazy, zeptejte se, stejně tak pokud je to zajímavé, pošlu fotografii. cenu 60.000. sleva je také možná</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/057/181258057.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181258057/volkswagen-passat-b6-20tdi.php</t>
+  </si>
+  <si>
+    <t>VOLKSWAGEN PASSAT 2.0TDI 103KW Koupeno ČR 2009</t>
+  </si>
+  <si>
+    <t>31.1. 2024</t>
+  </si>
+  <si>
+    <t>Koupeno Česká republika.pěkný stav-bez koroze.plná servisní kniha.počet ujetých kilometrů a stav tachometru je 228.900 km-Cebia Autotracer.motor cod CBA.Kombi.šestirychlostní manuál.Digi klima.výhřev sedaček.8x airbag.cd radio.zamykání řadící páky.dva klíče-centrál na dálku.el.parkovací brzda.el.okn ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/250/180637250.jpg?t=1706712136</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/180637250/volkswagen-passat-20tdi-103kw-koupeno-cr-2009.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2 1.6</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2.0 TDi -- Auto na splátky bez registru</t>
+  </si>
+  <si>
+    <t>Praha - východ 250 01</t>
+  </si>
+  <si>
+    <t>Minimální výše kauce: 45.000 Kč. Splátky: 7.900 x 36 Volejte: 731 721 902 Spolehlivá firma - Přes 8 let na trhu. Na splátky bez nahlížení do registru dlužníků a doložení příjmů. První splátka až měsíc po převzetí vozu. Motor: 1.6 TDi Převodovka: Manuální Rok výroby: 2014 Najeto: 250.000 ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/120/181392120.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181392120/skoda-octavia-20-tdi-auto-na-splatky-bez-registru.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2 combi 1.6 TDI 4x4</t>
+  </si>
+  <si>
+    <t>Česká Lípa 472 01</t>
+  </si>
+  <si>
+    <t>Škoda octavia 2 combi 1.6 TDI 4x4 Prodám Škoda octavia 2 combi 1.6 TDI 77 kW 4x4 6Q, rv. 2012, najeto 284k, vyhřívaná El. zrcátka, navi, sound systém, funkční klimatizace, 4x El okna, vyhřívané sedačky, multifunkční volant, bt přenos hudby, bt telefon, parkovací senzory vzadu, tažné zařízení, nové ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/592/178862592.jpg?t=1707583171</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/178862592/skoda-octavia-2-combi-16-tdi-4x4.php</t>
+  </si>
+  <si>
+    <t>Prodám Škoda Octavia 2</t>
+  </si>
+  <si>
+    <t>Přerov 751 31</t>
+  </si>
+  <si>
+    <t>Škoda octavia 2 se spolehlivým a úsporným naftovým motorem 1.6 TDI o výkonu 77kW. Rok výroby 2010. Manuální převodovka. Průměrná spotřeba 5 litrů. Stav tachometru 215.000 km Platná STK do 05/2025. Vůz plní EURO5, přepis jen 800 korun. Pravidelný servis, nové čerpadlo a vstřiky, rozvody. Veškeré fakt ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/317/178860317.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/178860317/prodam-skoda-octavia-2.php</t>
+  </si>
+  <si>
+    <t>Škoda octavia 2 facelift 1.9tdi</t>
+  </si>
+  <si>
+    <t>Praha 6 162 00</t>
+  </si>
+  <si>
+    <t>rodám škodu octavii 2 facelift 1.9tdi 77kw r.v.2010 najeto 300tis. Stk platná Výbava:el.okna,el.zrcátka,vyhřívaná zrcátka,vyhřívané sedačky,natáčecí xenony,dvouzonová clima,tempomat,palubní pc,originální radio s připojením na telefon,2 stínítka proti slunci Na aute dělaný před 30tis. Rozvody s ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/101/181303101.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181303101/skoda-octavia-2-facelift-19tdi.php</t>
+  </si>
+  <si>
+    <t>octavia 2 1.9 TDi 77kW combi verze bez DPF</t>
+  </si>
+  <si>
+    <t>10.2. 2024</t>
+  </si>
+  <si>
+    <t>Kroměříž 767 01</t>
+  </si>
+  <si>
+    <t>Dobry den, prodam skoda octavia 2 combi 1.9tdi 77kw rv. 2006,najeto 284xxxkm, zachovaly interier, vybava: centralni zamykani (2xdalkac) 4x el. okna, klima, el. zrcatka, loketni operka,abs, asr, airbag, tempomat, tonovana skla nove letni pneu 18 na litacich, nove zimni pneu 16, predni mlhovky,tazne ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/188/181125188.jpg?t=1707675862</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181125188/octavia-2-19-tdi-77kw-combi-verze-bez-dpf.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2 1.9 TDI 77kw BXE 2007</t>
+  </si>
+  <si>
+    <t>Prachatice 383 01</t>
+  </si>
+  <si>
+    <t>Prodám Octavii 2, 1.9 tdi 77kw BXE r.2007. Plně pojízdné. Najeto 302xxx km. Auto jsem měl na denní dojíždění do práce, vždy jsem udělal vše co bylo třeba. Komplet udělaný podvozek, vyměněný chladič, výměník oleje, nové turbo, spojka stará jeden rok, nové ložisko vpředu vlevo, rok staré brzdy včetně ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/644/179791644.jpg?t=1706271413</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/179791644/skoda-octavia-2-19-tdi-77kw-bxe-2007.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2.0 TDI DSG Combi Kůže Xenony Tažné</t>
+  </si>
+  <si>
+    <t>Praha 5 159 00</t>
+  </si>
+  <si>
+    <t>Škoda octavia II Combi se spolehlivým naftovým motorem 2.0 tdi o výkonu 103kW. Spotřeba 5,5 litrů. Automatická 6-ti stupňová převodovka. ALU R16 kola, zimní pneu s velmi dobrým vzorkem. Originální RS paket a černá stropnice. Rok výroby: 2005 Stav tachometru: 350.414 km - ověřené kilometry, Cebia rep ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/211/181542211.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181542211/skoda-octavia-20-tdi-dsg-combi-kuze-xenony-tazne.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2 2.0tdi 103kw 2007 Stk nová Tel:725 996 134</t>
+  </si>
+  <si>
+    <t>Vyškov 684 01</t>
+  </si>
+  <si>
+    <t>Dobrý den prodám auto značky Škoda octavia 2 2.0tdi 103kw rok výroby 2007 6kvalt... Možná i výměna ....Nabídněte ... Nová Stk ...... Najeto 430 000 ale rozvody dělaný ve 402 000,olej dělaný před 3000km.. Nyní před 9000km servis v podobě předních čepů,stabilizačních tyček,přední ramena, ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/439/181436439.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181436439/skoda-octavia-2-20tdi-103kw-2007-stk-nova-tel725-996-134.php</t>
+  </si>
+  <si>
+    <t>Škoda octavia 2.0TDI 103kw</t>
+  </si>
+  <si>
+    <t>Šumperk 789 01</t>
+  </si>
+  <si>
+    <t>Rok výroby 2005 Technická 6.2025 Šesti rychlostní převodovka Spotřeba 4,5-6L podle jízdy Po výměně olejů a filtrů Výbava : Tažné , vyhřívané přední sedačky , xenony, klimatizace atd. K vozidlu nechám ještě 2din autorádio . Obuto na zimních kolech . Interiér ve velmi pěkném stavu . Více ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/997/181421997.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181421997/skoda-octavia-20tdi-103kw.php</t>
+  </si>
+  <si>
+    <t>Minimální výše kauce: 45.000 Kč. Splátky: 7.900 x 36 Volejte: 731 721 902 Spolehlivá firma - Přes 8 let na trhu. Na splátky bez nahlížení do registru dlužníků a doložení příjmů. První splátka až měsíc po převzetí vozu. Motor: 1.6 tdi Převodovka: Manuální Rok výroby: 2014 Najeto: 250.000 ...</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2.0 TDi 6 rychl. po 1.maj. v ČR</t>
+  </si>
+  <si>
+    <t>Velmi dobrý stav, po jednom majiteli v ČR. K vozu všechny manuály, dva klíče, nová autobaterie. Vozidlo pravidelně servisované. Provoz: 03/2010 Palivo: nafta STK: 11/2025 Stav tachometru: 371 500 km Výkon: 103 kW VIN: TMBTEC1Z4AC013895 Výbava: 6ti rychlostní převodovka, 6xairbag, klimatiz ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/076/181333076.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181333076/skoda-octavia-20-tdi-6-rychl-po-1maj-v-cr.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2.0TDI</t>
+  </si>
+  <si>
+    <t>30.1. 2024</t>
+  </si>
+  <si>
+    <t>Škoda octavia 2.0tdi 103kw modelový rok 2005 ELEGANCE Typ motoru BKD, bez DPF z výroby Dovoz Německo, servisní kniha, najeto 197t km, 2 klíče Stk je nová v ČR, s autem je možné ihned odjet, vše funguje, jak má Digiklima, XENONY, kožený volant, tempomat, maxidot, parkovací senzory, vyhřívané seda ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/761/180566761.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/180566761/skoda-octavia-20tdi.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2 103Kw 2.0TDI BKD</t>
+  </si>
+  <si>
+    <t>21.1. 2024</t>
+  </si>
+  <si>
+    <t>Nabízím k prodeji druhou generaci Octavie, s autem stále jezdím tudíž kilometry stále přibývají. Má najeto 393tkm a je to 2.0tdi 103kw BKD. Bylo by v budoucnu vyměnit přední kotouče a brzdové destičky každopádně zatím to není nutné. Zadní brzdy jsou komplet nové tzn. destičky, kotouče, třmeny, měnil ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/366/180146366.jpg?t=1708194406</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/180146366/skoda-octavia-2-103kw-20tdi-bkd.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2.0 TDI,DSG,2008</t>
+  </si>
+  <si>
+    <t>12.1. 2024</t>
+  </si>
+  <si>
+    <t>Pelhřimov 394 46</t>
+  </si>
+  <si>
+    <t>Motor: 2.0 tdi (103 kw); Rok výroby: 2008 Najeto:320000km Převodovka: automatická DGS 6 stupňů Pohon: přední Bez filtru DPF z výroby Tažné zařízení Zařízení: • kožený interiér • vyhřívaná přední sedadla • Tempomat • kožený multifunkční volant, řazení pod volantem • palubní počítač ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/776/179696776.jpg?t=1705858111</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/179696776/skoda-octavia-20-tdidsg2008.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2.0 TDI 103KW po faceliftu</t>
+  </si>
+  <si>
+    <t>Kutná Hora 285 42</t>
+  </si>
+  <si>
+    <t>Prodám Škodu octavia 2 po faceliftu • Tažné zařízení • Xenony • Manuální převodovka 6 rychlostních stupňů • motor 103KW • Nafta/Diesel • Najeto 350xxx Km • Technická do do roku 24 ●VÝBAVA: Zadní parkovací senzory, vyhřívané zadní sklo, ABS, vyhřívané přední sedačky, tempomat, klimatizace, gu ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/702/178861702.jpg?t=1705318910</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/178861702/skoda-octavia-20-tdi-103kw-po-faceliftu.php</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181594872/koupim-skoda-fabia-i-ii-10-mpi-12-mpi-nebo-14-mpi.php</t>
+  </si>
+  <si>
+    <t>Škoda fabia</t>
+  </si>
+  <si>
+    <t>Havlíčkův Brod 582 44</t>
+  </si>
+  <si>
+    <t>Prodám Škodu fabii 1.4 mpi 44kw.stk do července.plne pojízdná bez investic,bez koroze.drobne oděrky a trochu promáčklé prah viz foto</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/021/181394021.jpg?t=1708321884</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181394021/skoda-fabia.php</t>
+  </si>
+  <si>
+    <t>ŠKODA FABIA 1.MAJITEL1.4MPi 50KW/ČR/PLNÝ SERVIS/TAŽNÉ ZAŘ.</t>
+  </si>
+  <si>
+    <t>Teplice 415 01</t>
+  </si>
+  <si>
+    <t>Prodám Škoda fabia. Rok výroby 2001. Motor osvědčená benzínová 1.4mpi o výkonu 50kw. Najeto podložených 271 tis.km. - interiér v hezkém, zachovalém stavu - karosérie v červené metalíze - mechanika v pořádku, k vozu držen pravidelný servis, vždy před pravidelnou STK prováděna větší údržba Výb ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/434/181343434.jpg?t=1708109156</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181343434/skoda-fabia-1majitel14mpi-50kwcrplny-servistazne-zar.php</t>
+  </si>
+  <si>
+    <t>Fabia I. 1.4Mpi</t>
+  </si>
+  <si>
+    <t>Kladno 272 01</t>
+  </si>
+  <si>
+    <t>Prodej automobilu Škoda fabia 1, rok výroby 2000 Značka a model: Škoda fabia 1 Motor: 1.4mpi Stav: Použité, s mírnými kosmetickými nedostatky Kilometrový stav: 110 890 km Vady: Čelní sklo má prasklinu způsobenou kamínkem, mírné poškrábání nad předním pravým kolem Vybavení: Zahrnuje jak zimní, tak l ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/835/181024835.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181024835/fabia-i-14mpi.php</t>
   </si>
 </sst>
 </file>
@@ -1452,7 +2064,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4AC74AD-538C-4782-8A8D-C4C0C7DD934D}">
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:M104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
@@ -3402,6 +4014,1810 @@
         <v>344</v>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>233</v>
+      </c>
+      <c r="B61" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C61" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D61" t="s">
+        <v>217</v>
+      </c>
+      <c r="E61" t="s">
+        <v>345</v>
+      </c>
+      <c r="F61" t="n">
+        <v>49000.0</v>
+      </c>
+      <c r="G61" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="H61" t="s">
+        <v>346</v>
+      </c>
+      <c r="I61" t="s">
+        <v>347</v>
+      </c>
+      <c r="J61" t="s">
+        <v>348</v>
+      </c>
+      <c r="K61" t="s">
+        <v>349</v>
+      </c>
+      <c r="L61" t="s">
+        <v>350</v>
+      </c>
+      <c r="M61" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>352</v>
+      </c>
+      <c r="B62" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C62" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D62" t="s">
+        <v>217</v>
+      </c>
+      <c r="E62" t="s">
+        <v>353</v>
+      </c>
+      <c r="F62" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="G62" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="H62" t="s">
+        <v>354</v>
+      </c>
+      <c r="I62" t="s">
+        <v>347</v>
+      </c>
+      <c r="J62" t="s">
+        <v>355</v>
+      </c>
+      <c r="K62" t="s">
+        <v>356</v>
+      </c>
+      <c r="L62" t="s">
+        <v>343</v>
+      </c>
+      <c r="M62" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>216</v>
+      </c>
+      <c r="B63" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C63" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D63" t="s">
+        <v>217</v>
+      </c>
+      <c r="E63" t="s">
+        <v>358</v>
+      </c>
+      <c r="F63" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="G63" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H63" t="s">
+        <v>220</v>
+      </c>
+      <c r="I63" t="s">
+        <v>347</v>
+      </c>
+      <c r="J63" t="s">
+        <v>359</v>
+      </c>
+      <c r="K63" t="s">
+        <v>360</v>
+      </c>
+      <c r="L63" t="s">
+        <v>361</v>
+      </c>
+      <c r="M63" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>216</v>
+      </c>
+      <c r="B64" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C64" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D64" t="s">
+        <v>217</v>
+      </c>
+      <c r="E64" t="s">
+        <v>353</v>
+      </c>
+      <c r="F64" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="G64" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="H64" t="s">
+        <v>354</v>
+      </c>
+      <c r="I64" t="s">
+        <v>347</v>
+      </c>
+      <c r="J64" t="s">
+        <v>355</v>
+      </c>
+      <c r="K64" t="s">
+        <v>356</v>
+      </c>
+      <c r="L64" t="s">
+        <v>343</v>
+      </c>
+      <c r="M64" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>225</v>
+      </c>
+      <c r="B65" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="C65" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D65" t="s">
+        <v>226</v>
+      </c>
+      <c r="E65" t="s">
+        <v>363</v>
+      </c>
+      <c r="F65" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="G65" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H65" t="s">
+        <v>235</v>
+      </c>
+      <c r="I65" t="s">
+        <v>347</v>
+      </c>
+      <c r="J65" t="s">
+        <v>364</v>
+      </c>
+      <c r="K65" t="s">
+        <v>365</v>
+      </c>
+      <c r="L65" t="s">
+        <v>366</v>
+      </c>
+      <c r="M65" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>225</v>
+      </c>
+      <c r="B66" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="C66" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D66" t="s">
+        <v>226</v>
+      </c>
+      <c r="E66" t="s">
+        <v>368</v>
+      </c>
+      <c r="F66" t="n">
+        <v>85000.0</v>
+      </c>
+      <c r="G66" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="H66" t="s">
+        <v>369</v>
+      </c>
+      <c r="I66" t="s">
+        <v>347</v>
+      </c>
+      <c r="J66" t="s">
+        <v>370</v>
+      </c>
+      <c r="K66" t="s">
+        <v>371</v>
+      </c>
+      <c r="L66" t="s">
+        <v>372</v>
+      </c>
+      <c r="M66" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>233</v>
+      </c>
+      <c r="B67" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="C67" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D67" t="s">
+        <v>217</v>
+      </c>
+      <c r="E67" t="s">
+        <v>374</v>
+      </c>
+      <c r="F67" t="n">
+        <v>60000.0</v>
+      </c>
+      <c r="G67" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H67" t="s">
+        <v>220</v>
+      </c>
+      <c r="I67" t="s">
+        <v>347</v>
+      </c>
+      <c r="J67" t="s">
+        <v>375</v>
+      </c>
+      <c r="K67" t="s">
+        <v>376</v>
+      </c>
+      <c r="L67" t="s">
+        <v>377</v>
+      </c>
+      <c r="M67" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>233</v>
+      </c>
+      <c r="B68" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="C68" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D68" t="s">
+        <v>217</v>
+      </c>
+      <c r="E68" t="s">
+        <v>345</v>
+      </c>
+      <c r="F68" t="n">
+        <v>49000.0</v>
+      </c>
+      <c r="G68" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="H68" t="s">
+        <v>346</v>
+      </c>
+      <c r="I68" t="s">
+        <v>347</v>
+      </c>
+      <c r="J68" t="s">
+        <v>348</v>
+      </c>
+      <c r="K68" t="s">
+        <v>349</v>
+      </c>
+      <c r="L68" t="s">
+        <v>379</v>
+      </c>
+      <c r="M68" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>246</v>
+      </c>
+      <c r="B69" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="C69" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D69" t="s">
+        <v>217</v>
+      </c>
+      <c r="E69" t="s">
+        <v>380</v>
+      </c>
+      <c r="F69" t="n">
+        <v>45000.0</v>
+      </c>
+      <c r="G69" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H69" t="s">
+        <v>220</v>
+      </c>
+      <c r="I69" t="s">
+        <v>347</v>
+      </c>
+      <c r="J69" t="s">
+        <v>249</v>
+      </c>
+      <c r="K69" t="s">
+        <v>381</v>
+      </c>
+      <c r="L69" t="s">
+        <v>382</v>
+      </c>
+      <c r="M69" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>246</v>
+      </c>
+      <c r="B70" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="C70" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D70" t="s">
+        <v>217</v>
+      </c>
+      <c r="E70" t="s">
+        <v>253</v>
+      </c>
+      <c r="F70" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="G70" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H70" t="s">
+        <v>220</v>
+      </c>
+      <c r="I70" t="s">
+        <v>347</v>
+      </c>
+      <c r="J70" t="s">
+        <v>255</v>
+      </c>
+      <c r="K70" t="s">
+        <v>384</v>
+      </c>
+      <c r="L70" t="s">
+        <v>385</v>
+      </c>
+      <c r="M70" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>246</v>
+      </c>
+      <c r="B71" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="C71" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D71" t="s">
+        <v>217</v>
+      </c>
+      <c r="E71" t="s">
+        <v>387</v>
+      </c>
+      <c r="F71" t="n">
+        <v>55000.0</v>
+      </c>
+      <c r="G71" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="H71" t="s">
+        <v>228</v>
+      </c>
+      <c r="I71" t="s">
+        <v>347</v>
+      </c>
+      <c r="J71" t="s">
+        <v>388</v>
+      </c>
+      <c r="K71" t="s">
+        <v>389</v>
+      </c>
+      <c r="L71" t="s">
+        <v>390</v>
+      </c>
+      <c r="M71" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>259</v>
+      </c>
+      <c r="B72" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C72" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D72" t="s">
+        <v>260</v>
+      </c>
+      <c r="E72" t="s">
+        <v>392</v>
+      </c>
+      <c r="F72" t="n">
+        <v>50000.0</v>
+      </c>
+      <c r="G72" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H72" t="s">
+        <v>220</v>
+      </c>
+      <c r="I72" t="s">
+        <v>347</v>
+      </c>
+      <c r="J72" t="s">
+        <v>393</v>
+      </c>
+      <c r="K72" t="s">
+        <v>394</v>
+      </c>
+      <c r="L72" t="s">
+        <v>395</v>
+      </c>
+      <c r="M72" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>259</v>
+      </c>
+      <c r="B73" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C73" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D73" t="s">
+        <v>260</v>
+      </c>
+      <c r="E73" t="s">
+        <v>397</v>
+      </c>
+      <c r="F73" t="n">
+        <v>58000.0</v>
+      </c>
+      <c r="G73" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H73" t="s">
+        <v>220</v>
+      </c>
+      <c r="I73" t="s">
+        <v>347</v>
+      </c>
+      <c r="J73" t="s">
+        <v>398</v>
+      </c>
+      <c r="K73" t="s">
+        <v>399</v>
+      </c>
+      <c r="L73" t="s">
+        <v>400</v>
+      </c>
+      <c r="M73" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>259</v>
+      </c>
+      <c r="B74" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C74" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D74" t="s">
+        <v>260</v>
+      </c>
+      <c r="E74" t="s">
+        <v>402</v>
+      </c>
+      <c r="F74" t="n">
+        <v>47000.0</v>
+      </c>
+      <c r="G74" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H74" t="s">
+        <v>220</v>
+      </c>
+      <c r="I74" t="s">
+        <v>347</v>
+      </c>
+      <c r="J74" t="s">
+        <v>268</v>
+      </c>
+      <c r="K74" t="s">
+        <v>269</v>
+      </c>
+      <c r="L74" t="s">
+        <v>403</v>
+      </c>
+      <c r="M74" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>259</v>
+      </c>
+      <c r="B75" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C75" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D75" t="s">
+        <v>260</v>
+      </c>
+      <c r="E75" t="s">
+        <v>405</v>
+      </c>
+      <c r="F75" t="n">
+        <v>85000.0</v>
+      </c>
+      <c r="G75" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H75" t="s">
+        <v>248</v>
+      </c>
+      <c r="I75" t="s">
+        <v>347</v>
+      </c>
+      <c r="J75" t="s">
+        <v>60</v>
+      </c>
+      <c r="K75" t="s">
+        <v>406</v>
+      </c>
+      <c r="L75" t="s">
+        <v>407</v>
+      </c>
+      <c r="M75" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>259</v>
+      </c>
+      <c r="B76" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C76" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D76" t="s">
+        <v>260</v>
+      </c>
+      <c r="E76" t="s">
+        <v>409</v>
+      </c>
+      <c r="F76" t="n">
+        <v>41111.0</v>
+      </c>
+      <c r="G76" t="n">
+        <v>61.0</v>
+      </c>
+      <c r="H76" t="s">
+        <v>410</v>
+      </c>
+      <c r="I76" t="s">
+        <v>347</v>
+      </c>
+      <c r="J76" t="s">
+        <v>411</v>
+      </c>
+      <c r="K76" t="s">
+        <v>412</v>
+      </c>
+      <c r="L76" t="s">
+        <v>413</v>
+      </c>
+      <c r="M76" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>278</v>
+      </c>
+      <c r="B77" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C77" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D77" t="s">
+        <v>260</v>
+      </c>
+      <c r="E77" t="s">
+        <v>415</v>
+      </c>
+      <c r="F77" t="n">
+        <v>63500.0</v>
+      </c>
+      <c r="G77" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H77" t="s">
+        <v>220</v>
+      </c>
+      <c r="I77" t="s">
+        <v>347</v>
+      </c>
+      <c r="J77" t="s">
+        <v>416</v>
+      </c>
+      <c r="K77" t="s">
+        <v>417</v>
+      </c>
+      <c r="L77" t="s">
+        <v>418</v>
+      </c>
+      <c r="M77" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>278</v>
+      </c>
+      <c r="B78" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C78" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D78" t="s">
+        <v>260</v>
+      </c>
+      <c r="E78" t="s">
+        <v>420</v>
+      </c>
+      <c r="F78" t="n">
+        <v>63000.0</v>
+      </c>
+      <c r="G78" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H78" t="s">
+        <v>220</v>
+      </c>
+      <c r="I78" t="s">
+        <v>347</v>
+      </c>
+      <c r="J78" t="s">
+        <v>66</v>
+      </c>
+      <c r="K78" t="s">
+        <v>421</v>
+      </c>
+      <c r="L78" t="s">
+        <v>422</v>
+      </c>
+      <c r="M78" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>278</v>
+      </c>
+      <c r="B79" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C79" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D79" t="s">
+        <v>260</v>
+      </c>
+      <c r="E79" t="s">
+        <v>424</v>
+      </c>
+      <c r="F79" t="n">
+        <v>63000.0</v>
+      </c>
+      <c r="G79" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H79" t="s">
+        <v>248</v>
+      </c>
+      <c r="I79" t="s">
+        <v>347</v>
+      </c>
+      <c r="J79" t="s">
+        <v>425</v>
+      </c>
+      <c r="K79" t="s">
+        <v>426</v>
+      </c>
+      <c r="L79" t="s">
+        <v>427</v>
+      </c>
+      <c r="M79" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>278</v>
+      </c>
+      <c r="B80" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C80" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D80" t="s">
+        <v>260</v>
+      </c>
+      <c r="E80" t="s">
+        <v>429</v>
+      </c>
+      <c r="F80" t="n">
+        <v>45000.0</v>
+      </c>
+      <c r="G80" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H80" t="s">
+        <v>248</v>
+      </c>
+      <c r="I80" t="s">
+        <v>347</v>
+      </c>
+      <c r="J80" t="s">
+        <v>430</v>
+      </c>
+      <c r="K80" t="s">
+        <v>431</v>
+      </c>
+      <c r="L80" t="s">
+        <v>432</v>
+      </c>
+      <c r="M80" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>278</v>
+      </c>
+      <c r="B81" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C81" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D81" t="s">
+        <v>260</v>
+      </c>
+      <c r="E81" t="s">
+        <v>434</v>
+      </c>
+      <c r="F81" t="n">
+        <v>87000.0</v>
+      </c>
+      <c r="G81" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="H81" t="s">
+        <v>228</v>
+      </c>
+      <c r="I81" t="s">
+        <v>347</v>
+      </c>
+      <c r="J81" t="s">
+        <v>435</v>
+      </c>
+      <c r="K81" t="s">
+        <v>436</v>
+      </c>
+      <c r="L81" t="s">
+        <v>437</v>
+      </c>
+      <c r="M81" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>278</v>
+      </c>
+      <c r="B82" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C82" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D82" t="s">
+        <v>260</v>
+      </c>
+      <c r="E82" t="s">
+        <v>439</v>
+      </c>
+      <c r="F82" t="n">
+        <v>55000.0</v>
+      </c>
+      <c r="G82" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="H82" t="s">
+        <v>273</v>
+      </c>
+      <c r="I82" t="s">
+        <v>347</v>
+      </c>
+      <c r="J82" t="s">
+        <v>440</v>
+      </c>
+      <c r="K82" t="s">
+        <v>441</v>
+      </c>
+      <c r="L82" t="s">
+        <v>442</v>
+      </c>
+      <c r="M82" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>278</v>
+      </c>
+      <c r="B83" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C83" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D83" t="s">
+        <v>260</v>
+      </c>
+      <c r="E83" t="s">
+        <v>444</v>
+      </c>
+      <c r="F83" t="n">
+        <v>75000.0</v>
+      </c>
+      <c r="G83" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="H83" t="s">
+        <v>445</v>
+      </c>
+      <c r="I83" t="s">
+        <v>347</v>
+      </c>
+      <c r="J83" t="s">
+        <v>446</v>
+      </c>
+      <c r="K83" t="s">
+        <v>447</v>
+      </c>
+      <c r="L83" t="s">
+        <v>448</v>
+      </c>
+      <c r="M83" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>278</v>
+      </c>
+      <c r="B84" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C84" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D84" t="s">
+        <v>260</v>
+      </c>
+      <c r="E84" t="s">
+        <v>450</v>
+      </c>
+      <c r="F84" t="n">
+        <v>60000.0</v>
+      </c>
+      <c r="G84" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="H84" t="s">
+        <v>451</v>
+      </c>
+      <c r="I84" t="s">
+        <v>347</v>
+      </c>
+      <c r="J84" t="s">
+        <v>268</v>
+      </c>
+      <c r="K84" t="s">
+        <v>452</v>
+      </c>
+      <c r="L84" t="s">
+        <v>453</v>
+      </c>
+      <c r="M84" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>278</v>
+      </c>
+      <c r="B85" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C85" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D85" t="s">
+        <v>260</v>
+      </c>
+      <c r="E85" t="s">
+        <v>455</v>
+      </c>
+      <c r="F85" t="n">
+        <v>96000.0</v>
+      </c>
+      <c r="G85" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="H85" t="s">
+        <v>456</v>
+      </c>
+      <c r="I85" t="s">
+        <v>347</v>
+      </c>
+      <c r="J85" t="s">
+        <v>388</v>
+      </c>
+      <c r="K85" t="s">
+        <v>457</v>
+      </c>
+      <c r="L85" t="s">
+        <v>458</v>
+      </c>
+      <c r="M85" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>460</v>
+      </c>
+      <c r="B86" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C86" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D86" t="s">
+        <v>191</v>
+      </c>
+      <c r="E86" t="s">
+        <v>461</v>
+      </c>
+      <c r="F86" t="n">
+        <v>45000.0</v>
+      </c>
+      <c r="G86" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="H86" t="s">
+        <v>228</v>
+      </c>
+      <c r="I86" t="s">
+        <v>347</v>
+      </c>
+      <c r="J86" t="s">
+        <v>462</v>
+      </c>
+      <c r="K86" t="s">
+        <v>463</v>
+      </c>
+      <c r="L86" t="s">
+        <v>464</v>
+      </c>
+      <c r="M86" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>460</v>
+      </c>
+      <c r="B87" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C87" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D87" t="s">
+        <v>191</v>
+      </c>
+      <c r="E87" t="s">
+        <v>466</v>
+      </c>
+      <c r="F87" t="n">
+        <v>95000.0</v>
+      </c>
+      <c r="G87" t="n">
+        <v>61.0</v>
+      </c>
+      <c r="H87" t="s">
+        <v>410</v>
+      </c>
+      <c r="I87" t="s">
+        <v>347</v>
+      </c>
+      <c r="J87" t="s">
+        <v>467</v>
+      </c>
+      <c r="K87" t="s">
+        <v>468</v>
+      </c>
+      <c r="L87" t="s">
+        <v>469</v>
+      </c>
+      <c r="M87" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>460</v>
+      </c>
+      <c r="B88" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C88" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D88" t="s">
+        <v>191</v>
+      </c>
+      <c r="E88" t="s">
+        <v>471</v>
+      </c>
+      <c r="F88" t="n">
+        <v>90000.0</v>
+      </c>
+      <c r="G88" t="n">
+        <v>61.0</v>
+      </c>
+      <c r="H88" t="s">
+        <v>410</v>
+      </c>
+      <c r="I88" t="s">
+        <v>347</v>
+      </c>
+      <c r="J88" t="s">
+        <v>472</v>
+      </c>
+      <c r="K88" t="s">
+        <v>473</v>
+      </c>
+      <c r="L88" t="s">
+        <v>474</v>
+      </c>
+      <c r="M88" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>302</v>
+      </c>
+      <c r="B89" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C89" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D89" t="s">
+        <v>191</v>
+      </c>
+      <c r="E89" t="s">
+        <v>476</v>
+      </c>
+      <c r="F89" t="n">
+        <v>99000.0</v>
+      </c>
+      <c r="G89" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="H89" t="s">
+        <v>445</v>
+      </c>
+      <c r="I89" t="s">
+        <v>347</v>
+      </c>
+      <c r="J89" t="s">
+        <v>477</v>
+      </c>
+      <c r="K89" t="s">
+        <v>478</v>
+      </c>
+      <c r="L89" t="s">
+        <v>479</v>
+      </c>
+      <c r="M89" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>302</v>
+      </c>
+      <c r="B90" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C90" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D90" t="s">
+        <v>191</v>
+      </c>
+      <c r="E90" t="s">
+        <v>481</v>
+      </c>
+      <c r="F90" t="n">
+        <v>80000.0</v>
+      </c>
+      <c r="G90" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="H90" t="s">
+        <v>482</v>
+      </c>
+      <c r="I90" t="s">
+        <v>347</v>
+      </c>
+      <c r="J90" t="s">
+        <v>483</v>
+      </c>
+      <c r="K90" t="s">
+        <v>484</v>
+      </c>
+      <c r="L90" t="s">
+        <v>485</v>
+      </c>
+      <c r="M90" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>302</v>
+      </c>
+      <c r="B91" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C91" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D91" t="s">
+        <v>191</v>
+      </c>
+      <c r="E91" t="s">
+        <v>487</v>
+      </c>
+      <c r="F91" t="n">
+        <v>65000.0</v>
+      </c>
+      <c r="G91" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="H91" t="s">
+        <v>327</v>
+      </c>
+      <c r="I91" t="s">
+        <v>347</v>
+      </c>
+      <c r="J91" t="s">
+        <v>488</v>
+      </c>
+      <c r="K91" t="s">
+        <v>489</v>
+      </c>
+      <c r="L91" t="s">
+        <v>490</v>
+      </c>
+      <c r="M91" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>332</v>
+      </c>
+      <c r="B92" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C92" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D92" t="s">
+        <v>191</v>
+      </c>
+      <c r="E92" t="s">
+        <v>492</v>
+      </c>
+      <c r="F92" t="n">
+        <v>79900.0</v>
+      </c>
+      <c r="G92" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H92" t="s">
+        <v>248</v>
+      </c>
+      <c r="I92" t="s">
+        <v>347</v>
+      </c>
+      <c r="J92" t="s">
+        <v>493</v>
+      </c>
+      <c r="K92" t="s">
+        <v>494</v>
+      </c>
+      <c r="L92" t="s">
+        <v>495</v>
+      </c>
+      <c r="M92" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>332</v>
+      </c>
+      <c r="B93" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C93" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D93" t="s">
+        <v>191</v>
+      </c>
+      <c r="E93" t="s">
+        <v>497</v>
+      </c>
+      <c r="F93" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="G93" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H93" t="s">
+        <v>267</v>
+      </c>
+      <c r="I93" t="s">
+        <v>347</v>
+      </c>
+      <c r="J93" t="s">
+        <v>498</v>
+      </c>
+      <c r="K93" t="s">
+        <v>499</v>
+      </c>
+      <c r="L93" t="s">
+        <v>500</v>
+      </c>
+      <c r="M93" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>332</v>
+      </c>
+      <c r="B94" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C94" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D94" t="s">
+        <v>191</v>
+      </c>
+      <c r="E94" t="s">
+        <v>502</v>
+      </c>
+      <c r="F94" t="n">
+        <v>60000.0</v>
+      </c>
+      <c r="G94" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H94" t="s">
+        <v>267</v>
+      </c>
+      <c r="I94" t="s">
+        <v>347</v>
+      </c>
+      <c r="J94" t="s">
+        <v>503</v>
+      </c>
+      <c r="K94" t="s">
+        <v>504</v>
+      </c>
+      <c r="L94" t="s">
+        <v>505</v>
+      </c>
+      <c r="M94" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>332</v>
+      </c>
+      <c r="B95" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C95" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D95" t="s">
+        <v>191</v>
+      </c>
+      <c r="E95" t="s">
+        <v>461</v>
+      </c>
+      <c r="F95" t="n">
+        <v>45000.0</v>
+      </c>
+      <c r="G95" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="H95" t="s">
+        <v>228</v>
+      </c>
+      <c r="I95" t="s">
+        <v>347</v>
+      </c>
+      <c r="J95" t="s">
+        <v>462</v>
+      </c>
+      <c r="K95" t="s">
+        <v>507</v>
+      </c>
+      <c r="L95" t="s">
+        <v>464</v>
+      </c>
+      <c r="M95" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>332</v>
+      </c>
+      <c r="B96" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C96" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D96" t="s">
+        <v>191</v>
+      </c>
+      <c r="E96" t="s">
+        <v>508</v>
+      </c>
+      <c r="F96" t="n">
+        <v>95999.0</v>
+      </c>
+      <c r="G96" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="H96" t="s">
+        <v>273</v>
+      </c>
+      <c r="I96" t="s">
+        <v>347</v>
+      </c>
+      <c r="J96" t="s">
+        <v>26</v>
+      </c>
+      <c r="K96" t="s">
+        <v>509</v>
+      </c>
+      <c r="L96" t="s">
+        <v>510</v>
+      </c>
+      <c r="M96" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>332</v>
+      </c>
+      <c r="B97" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C97" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D97" t="s">
+        <v>191</v>
+      </c>
+      <c r="E97" t="s">
+        <v>512</v>
+      </c>
+      <c r="F97" t="n">
+        <v>99900.0</v>
+      </c>
+      <c r="G97" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="H97" t="s">
+        <v>513</v>
+      </c>
+      <c r="I97" t="s">
+        <v>347</v>
+      </c>
+      <c r="J97" t="s">
+        <v>195</v>
+      </c>
+      <c r="K97" t="s">
+        <v>514</v>
+      </c>
+      <c r="L97" t="s">
+        <v>515</v>
+      </c>
+      <c r="M97" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>332</v>
+      </c>
+      <c r="B98" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C98" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D98" t="s">
+        <v>191</v>
+      </c>
+      <c r="E98" t="s">
+        <v>517</v>
+      </c>
+      <c r="F98" t="n">
+        <v>59000.0</v>
+      </c>
+      <c r="G98" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="H98" t="s">
+        <v>518</v>
+      </c>
+      <c r="I98" t="s">
+        <v>347</v>
+      </c>
+      <c r="J98" t="s">
+        <v>66</v>
+      </c>
+      <c r="K98" t="s">
+        <v>519</v>
+      </c>
+      <c r="L98" t="s">
+        <v>520</v>
+      </c>
+      <c r="M98" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>332</v>
+      </c>
+      <c r="B99" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C99" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D99" t="s">
+        <v>191</v>
+      </c>
+      <c r="E99" t="s">
+        <v>522</v>
+      </c>
+      <c r="F99" t="n">
+        <v>95000.0</v>
+      </c>
+      <c r="G99" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="H99" t="s">
+        <v>523</v>
+      </c>
+      <c r="I99" t="s">
+        <v>347</v>
+      </c>
+      <c r="J99" t="s">
+        <v>524</v>
+      </c>
+      <c r="K99" t="s">
+        <v>525</v>
+      </c>
+      <c r="L99" t="s">
+        <v>526</v>
+      </c>
+      <c r="M99" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>332</v>
+      </c>
+      <c r="B100" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C100" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D100" t="s">
+        <v>191</v>
+      </c>
+      <c r="E100" t="s">
+        <v>528</v>
+      </c>
+      <c r="F100" t="n">
+        <v>80000.0</v>
+      </c>
+      <c r="G100" t="n">
+        <v>61.0</v>
+      </c>
+      <c r="H100" t="s">
+        <v>410</v>
+      </c>
+      <c r="I100" t="s">
+        <v>347</v>
+      </c>
+      <c r="J100" t="s">
+        <v>529</v>
+      </c>
+      <c r="K100" t="s">
+        <v>530</v>
+      </c>
+      <c r="L100" t="s">
+        <v>531</v>
+      </c>
+      <c r="M100" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>338</v>
+      </c>
+      <c r="B101" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="C101" t="n">
+        <v>35000.0</v>
+      </c>
+      <c r="D101" t="s">
+        <v>339</v>
+      </c>
+      <c r="E101" t="s">
+        <v>340</v>
+      </c>
+      <c r="F101" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="G101" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H101" t="s">
+        <v>220</v>
+      </c>
+      <c r="I101" t="s">
+        <v>347</v>
+      </c>
+      <c r="J101" t="s">
+        <v>341</v>
+      </c>
+      <c r="K101" t="s">
+        <v>342</v>
+      </c>
+      <c r="L101" t="s">
+        <v>343</v>
+      </c>
+      <c r="M101" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>338</v>
+      </c>
+      <c r="B102" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="C102" t="n">
+        <v>35000.0</v>
+      </c>
+      <c r="D102" t="s">
+        <v>339</v>
+      </c>
+      <c r="E102" t="s">
+        <v>534</v>
+      </c>
+      <c r="F102" t="n">
+        <v>22000.0</v>
+      </c>
+      <c r="G102" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="H102" t="s">
+        <v>228</v>
+      </c>
+      <c r="I102" t="s">
+        <v>347</v>
+      </c>
+      <c r="J102" t="s">
+        <v>535</v>
+      </c>
+      <c r="K102" t="s">
+        <v>536</v>
+      </c>
+      <c r="L102" t="s">
+        <v>537</v>
+      </c>
+      <c r="M102" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>338</v>
+      </c>
+      <c r="B103" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="C103" t="n">
+        <v>35000.0</v>
+      </c>
+      <c r="D103" t="s">
+        <v>339</v>
+      </c>
+      <c r="E103" t="s">
+        <v>539</v>
+      </c>
+      <c r="F103" t="n">
+        <v>27000.0</v>
+      </c>
+      <c r="G103" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="H103" t="s">
+        <v>273</v>
+      </c>
+      <c r="I103" t="s">
+        <v>347</v>
+      </c>
+      <c r="J103" t="s">
+        <v>540</v>
+      </c>
+      <c r="K103" t="s">
+        <v>541</v>
+      </c>
+      <c r="L103" t="s">
+        <v>542</v>
+      </c>
+      <c r="M103" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>338</v>
+      </c>
+      <c r="B104" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="C104" t="n">
+        <v>35000.0</v>
+      </c>
+      <c r="D104" t="s">
+        <v>339</v>
+      </c>
+      <c r="E104" t="s">
+        <v>544</v>
+      </c>
+      <c r="F104" t="n">
+        <v>25000.0</v>
+      </c>
+      <c r="G104" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="H104" t="s">
+        <v>304</v>
+      </c>
+      <c r="I104" t="s">
+        <v>347</v>
+      </c>
+      <c r="J104" t="s">
+        <v>545</v>
+      </c>
+      <c r="K104" t="s">
+        <v>546</v>
+      </c>
+      <c r="L104" t="s">
+        <v>547</v>
+      </c>
+      <c r="M104" t="s">
+        <v>548</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Přidání delaye pro použití metody isCar
</commit_message>
<xml_diff>
--- a/prodeje.xlsx
+++ b/prodeje.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1748" uniqueCount="1036">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2122" uniqueCount="1201">
   <si>
     <t>Item</t>
   </si>
@@ -3144,6 +3144,501 @@
   </si>
   <si>
     <t>https://auto.bazos.cz/inzerat/179057054/skoda-fabia-14-mpi.php</t>
+  </si>
+  <si>
+    <t>Prodám bmw 320d e46</t>
+  </si>
+  <si>
+    <t>28.2. 2024</t>
+  </si>
+  <si>
+    <t>Liberec 463 53</t>
+  </si>
+  <si>
+    <t>Prodám: bmw e46 Touring RV. - 2005 facelift Vykon -110kw Razení - 6q manuál Najeto - 306xxx Dnes auto po servisů víc jak 35 tisíc Tazné zařízení Alu kola R16 Cerná stropnice Multi.volant Zadni senzory - pdc El okna El.zrcátka ESP, ABS Stk 11/24 Vyhrivané sedačky Tempomat Changer CD Klíma Nova řeme ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/943/181080943.jpg?t=1709018257</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181080943/prodam-bmw-320d-e46.php</t>
+  </si>
+  <si>
+    <t>BMW 320 d</t>
+  </si>
+  <si>
+    <t>Vyškov 682 01</t>
+  </si>
+  <si>
+    <t>Prodám bmw e46 320d 110 kw automat. Nájezd: 341xxx km Automat řadí plynule Vůz je po servisu: palivový filtr, vzduchový a kabinový filtr, výměna oleje a olejového filtru, výměna vodní pumpy, termostatu a klínového řemene, nové stahovačky oken Výbava: vyhřívané přední sedačky, tempomat, multifu ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/534/180096534.jpg?t=1708407511</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/180096534/bmw-320-d.php</t>
+  </si>
+  <si>
+    <t>26.2. 2024</t>
+  </si>
+  <si>
+    <t>Zdravím, prodám bmw e46 320d 110kw 6q. Rok výroby 2004, počet najetých km 329 000km. Jedná se o originální tovární m-paket, žádná předělávka. Vozidlo po servise za 4000 euro-nová spojka, repas motoru a další faktury mám. Servisní knížka také vedena. Aktuálně po nové dovozové STK plátna do 1/2026 při ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/197/181891197.jpg?t=1708981506</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181891197/bmw-e46-320d-110kw.php</t>
+  </si>
+  <si>
+    <t>Bmw 320d 110kw</t>
+  </si>
+  <si>
+    <t>23.2. 2024</t>
+  </si>
+  <si>
+    <t>Nabízím k prodeji bmw e46 320d 110kw touring se spolehlivým a úsporným motorem m47 a šestistupňovou převodovkou manuální, rok výroby 2003, Stk do 05/2024.Spotřeba 5,5L. Výbava -El.okna v předu,Černa stropnice, multifunkční volant,alu zimní r16 ,2xklíč ,dešťový senzor. Byli dělaný věci: al ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/677/180508677.jpg?t=1708637345</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/180508677/bmw-320d-110kw.php</t>
+  </si>
+  <si>
+    <t>Prodám nebo vyměním e46 320d</t>
+  </si>
+  <si>
+    <t>24.2. 2024</t>
+  </si>
+  <si>
+    <t>Olomouc 783 01</t>
+  </si>
+  <si>
+    <t>Prodám nebo vyměním bmw e46 320d 100kw Nájezd 271xxy Stk platná na dva roky Auto plně pojízdné a Funkční tichý a pravidelní chod motorů žádný únik kapalin.. Auto tahá pěkně od spodu Na autě proběhla klasická výměna oleje a filtrů Brzdy Podvozek Majitel před dělal těsnění pod hlavou ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/229/181778229.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181778229/prodam-nebo-vymenim-e46-320d.php</t>
+  </si>
+  <si>
+    <t>BMW 328i Touring</t>
+  </si>
+  <si>
+    <t>Jihlava 586 01</t>
+  </si>
+  <si>
+    <t>Chtěl bych nabídnout k prodeji svoji e46 328i Touring s manuálem. Je to rok výroby 2000, má najeto něco málo přes 296 tisíc. Auto jsem kupoval na konci listopadu kvůli tomu, že druhou zadokolku jsem měl rozebranou a mělo slušně napadnout. S autem jsem od té doby najel asi 700 kilometrů (dva dny n ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/785/181260785.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181260785/bmw-328i-touring.php</t>
+  </si>
+  <si>
+    <t>Volkswagen Passat 1.9 TDI 96KW 6kavlt facelift R.V 2005</t>
+  </si>
+  <si>
+    <t>Prodám volkswagen passat 1.9 tdi 96KW 6 stupňová manuální převodovka Rok výroby 2005 Koupený V ČR Najeto 257 000 KM poctive 12 let jeden majitel Výbava El okna El zrcátka digitální klimatizace tempomat vyhřívaná sedadla palubní počítač 2x klíč a mnoha dalšího Vůz jezdí krásně a bez problémů a jeto ...</t>
+  </si>
+  <si>
+    <t>https://cdn.discordapp.com/attachments/1063949035054051409/1212073653328416848/Volkswagen_Passat_1.9_TDI_96KW_6kavlt_facelift_R.V_2005.jpg?ex=65f0828e&amp;is=65de0d8e&amp;hm=803bf829f04cc6cc83103fddd5d8133cf21338cbbc036b0b834aa161d5e72fe5&amp;</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181917793/volkswagen-passat-19-tdi-96kw-6kavlt-facelift-rv-2005.php</t>
+  </si>
+  <si>
+    <t>Volkswagen Passat 1.9TDI 77Kw</t>
+  </si>
+  <si>
+    <t>Ústí nad Labem 400 03</t>
+  </si>
+  <si>
+    <t>VW passat B6 Prodám passat B6 1.9 tdi 77kw Model 2007 Najeto 249xxx Digitální klimatizace Abs servo centrál Navigační systém 2x klíč jezdí skvěle. 3 měsíce zpátky bylo děláno turbo. Auto je v dobrém technickém stavu. STK do 14.6 2025. Dle stavu zohledněna cena</t>
+  </si>
+  <si>
+    <t>https://cdn.discordapp.com/attachments/1063949035054051409/1212073686819934279/Volkswagen_Passat_1.9TDI_77Kw.jpg?ex=65f08296&amp;is=65de0d96&amp;hm=36989aa76e79f7957209afac067a1c6de532185453ce27f98fcc8c473c17df7b&amp;</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181726977/volkswagen-passat-19tdi-77kw.php</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/959/181921959.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181921959/volkswagen-passat-variant-20tdi-103-kw-aut-klima.php</t>
+  </si>
+  <si>
+    <t>Volkswagen Passat Variant 2.0TDI,Highline,Bez DPF</t>
+  </si>
+  <si>
+    <t>Prodám passat B6,2006 Bez DPF s platnou STK do 6.2025 najeto 260000km.Je to manuál 6kvalt.Výbava Highline Bi-xenony naklápění a přísvícení do zatáček,okna zrcátka v el.vcetně předních sedaček a všechny sedačky mají funkční výhřev a jsou klimatizované,tempomat a další je toho moc to sem vypisovat.Int ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/020/181901020.jpg?t=1709015148</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181901020/volkswagen-passat-variant-20tdihighlinebez-dpf.php</t>
+  </si>
+  <si>
+    <t>Volkswagen Passat, 2.0 TDI, 4motion Highline</t>
+  </si>
+  <si>
+    <t>30.12. 2023</t>
+  </si>
+  <si>
+    <t>volkswagen passat, 2.0 tdi, 4motion Highline, r.v 2007 najeto 304000km, stk do 11/25, bez dpf filtru. Na podzim nové brzdové motůrky ruční brzdy, ve 294000km nové rozvody, 304600km výměna oleje. Výbava: Kožené čalounění, Imobilizér, ABS, El. ovládání zrcátek, ESP, Tempomat, Dálkové centrální zamy ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/122/179110122.jpg?t=1708273484</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/179110122/volkswagen-passat-20-tdi-4motion-highline.php</t>
+  </si>
+  <si>
+    <t>Brno venkov 594 55</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/395/181786395.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181786395/skoda-octavia-16-mpi-75kw-najezd-158tis.php</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/778/181748778.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181748778/skoda-octavia-16-mpi-75kw.php</t>
+  </si>
+  <si>
+    <t>Škoda octavia 2 1.6 mpi</t>
+  </si>
+  <si>
+    <t>Jičín 508 01</t>
+  </si>
+  <si>
+    <t>Škoda octavia 2 1.6 mpi 75kw Rv 04 najeto 166tis ve 135tis dělané rozvody. STK do 6.2024 3 majitel v ČR Výroba Mladá Boleslav Vybava. Pal pc Tempomat 2zonova digi clima 4x el okna El zrcátka Central dálka Asr 2xklic Obuta na zimnich pneu Podvozek tuhý bez vůle Brzdy spojka ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/839/181692839.jpg?t=1708889167</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181692839/skoda-octavia-2-16-mpi.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 1.6 77kw</t>
+  </si>
+  <si>
+    <t>Ústí nad Orlicí 561 55</t>
+  </si>
+  <si>
+    <t>Prodám škoda octavia 2 1.6 77kw,po jednom majiteli,najeto 150000km,okna v elektrice,centrál,klimatizace, servisní knížka, 3xklic, čerstvá stk,zachovaly a udržovaný vůz,majitel prodal auto z důvodu svého věku už musel odevzdat řidičák pro to je to top stav,stále garazovany, jen vážni zájemci prosím,n ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/520/181393520.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181393520/skoda-octavia-16-77kw.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2 1.9tdi 77kw 2005 bez DPF manuál</t>
+  </si>
+  <si>
+    <t>Škoda octavia 2 Přelom 2005 Kód motoru: BJB - bez DPF z výroby Nájezd:460tkm - motor běží tiše Obsah: 1.9tdi 77kw Palivo: Nafta Spotřeba: 4.8L Převodovka: Manuální STK: 2025/11 Přepis Pouze 800kč Nájezd na autě není vůbec znát,Motor je v perfektním stavu běží tiše, turbo táhne dobře řekl ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/637/181879637.jpg?t=1708964547</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181879637/skoda-octavia-2-19tdi-77kw-2005-bez-dpf-manual.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2 1.9TDI 77kw</t>
+  </si>
+  <si>
+    <t>Prodám octavia II 1.9 tdi 77KW Vozidlo je plně pojizdné v dobrém technickém stavu. Na vozidle nesvítí žádná chybová kontrolka a jezdí normálně. Na vozidle jsou ALU R15 se zánovním zimním pneu Continental. Motor 1.9tdi 77kw (bez DPF) Převodovka 5st. manuál Usporné, pohodlné a spolehlivé ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/292/181813292.jpg?t=1708872584</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181813292/skoda-octavia-2-19tdi-77kw.php</t>
+  </si>
+  <si>
+    <t>Škoda octavie 2</t>
+  </si>
+  <si>
+    <t>Praha - východ 251 01</t>
+  </si>
+  <si>
+    <t>Prodám vůz Škoda octavia 2 s motorizací 1.9 tdi s výkonem 77kw a pětistupňovou manuální převodovkou. Motor: 1.9 tdi 77kw Rok výroby: 2007 Stav tachometru: 444.382km STK: 09/25 Výbava: klimatizace, tempomat, tažné zařízení. Servis: spojka, prahy, blatníky, homo. kloub. Auto zachovalé v pěkné ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/181/181908181.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181908181/skoda-octavie-2.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2 1.9tdi 77kw</t>
+  </si>
+  <si>
+    <t>Dobrý den. Nabízím naší rodinou Octavii 2 COMBI 1.9 tdi 77kw, motor BJB, rok 2005 AMBIENTE . Auto denně v provozu , najeto 309540km. Něco k autu nyní nová přední světla asi měsíc stará svítí skvěle , v loni kompresor klimatizace DENZO nový chladič klimatizace + náplň + čidlo. Nové pružiny přední ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/420/181879420.jpg?t=1708964819</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181879420/skoda-octavia-2-19tdi-77kw.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia II 1.9tdi 77kw</t>
+  </si>
+  <si>
+    <t>Praha - východ 250 81</t>
+  </si>
+  <si>
+    <t>Prodám skoda octavia 2, obsah 1.9tdi 77kw, rok 2005, najeto poctivých 283.000km, 2.majitel koupeno v ČR, barva stříbrná metalíza, platná stk, pravidelně servisováno oleje a filtry, po motorové stránce super, kosmetické vady s běžného provozu, krásný interiér, Výbava:dálkové zamykání,manuální převo ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/449/181776449.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181776449/skoda-octavia-ii-19tdi-77kw.php</t>
+  </si>
+  <si>
+    <t>Prodam Škoda octavia 2 1.9tdi</t>
+  </si>
+  <si>
+    <t>Brno venkov 691 23</t>
+  </si>
+  <si>
+    <t>Prodam Škoda octavia 2 elegance 1.9tdi 77kw 2005 nova stk nový motor najeto 280tis km nove rozvody před 3 měsícemi novy olej filtry čepy stabilizační tičky ramena zadni uloženi tlumiču pružiny octavia 2 rs předni zadni naraznik rs vybava tempomat vyhřev sedaček zrcatek el zrcatka el okna 4x. Palub ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/927/181455927.jpg?t=1708771813</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181455927/prodam-skoda-octavia-2-19tdi.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 1.9 77kw</t>
+  </si>
+  <si>
+    <t>Teplice 417 13</t>
+  </si>
+  <si>
+    <t>Prodám Škodu octavia 2005 s motorem 1.9 tdi modrá metalíza .Výbava ABS,asr,klima,el.okna Central,tažné zařízení.Jedna se o dovoz po dohodě nová stk</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/047/181394047.jpg?t=1708080804</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181394047/skoda-octavia-19-77kw.php</t>
+  </si>
+  <si>
+    <t>Škoda octavia 2 Fl. 1.9tdi 77kw 2010</t>
+  </si>
+  <si>
+    <t>Mělník 277 32</t>
+  </si>
+  <si>
+    <t>Dobrý den,prodám Škoda octavia 2 facelift 1.9 tdi 77kw rok výroby 2010 najeto 405XXX Na autě je potřeba udělat palivová pumpa,ozývá se dvouhmota ale zatím jen za studena. Auto je po srážce ze srnou ale neodborně opraveno (byla vyměněna kapota,světla,přední nárazník a maska. Před 14 dny nový olej, ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/989/180930989.jpg?t=1707294112</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/180930989/skoda-octavia-2-fl-19tdi-77kw-2010.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2.0 TDI, RS 125 KW</t>
+  </si>
+  <si>
+    <t>Šumperk 787 01</t>
+  </si>
+  <si>
+    <t>ŠKODA octavia RS 125KW COMBI, ROK VÝROBY 2007, MANUÁLNÍ PŘEVODOVKA Prodám spolehlivý a výkonný vůz ŠKODA octavia RS s kombinovanou výbavou a sportovním designem. Tato verze nabízí skvělý výkon a zároveň pohodlí pro každodenní používání. TECHNICKÉ ÚDAJE: Motor: 125KW Převodovka: Manuální ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/579/180736579.jpg?t=1708538668</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/180736579/skoda-octavia-rs-125kw-combi-rok-vyroby-2007-manualni-prev.php</t>
+  </si>
+  <si>
+    <t>Prodám Škoda Octavia 2.0 TDI 103 kW plus soft</t>
+  </si>
+  <si>
+    <t>Jičín 507 24</t>
+  </si>
+  <si>
+    <t>Prodám Škoda octavia 2.0 tdi najeto 272 tisíc základ 103 kW plus soft na 138 kW jede úžasné ,vůz je po velkém servisu za cca 35 tisíc ,nové turbo oleje brzdy ložiska tlumiče víc přikládám foto, vybavení 4x El okna klimatizace dešťový senzor vyhřívané sedačky palubní počítač tempomat centrál na do,dv ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/026/181722026.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181722026/prodam-skoda-octavia-20-tdi-103-kw-plus-soft.php</t>
+  </si>
+  <si>
+    <t>Prodám Škoda Octavia 2.0 tdi</t>
+  </si>
+  <si>
+    <t>Prodám Škoda octavia 2.0 tdi 103kw. R.v.2005 STK 6/2025 10x airbag 6 rychlostni Naj.314tis.km Xenony Vyhřívané sedačky Sound systém Tempomat Dvouzónová klimatizace 4x elektrika oken Senzor dešte stěračů 2xklič s dálkovým. Dvojité dno v kufru. Servisovane,není momentálně žádné investice. Rozvody naj ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/423/181641423.jpg?t=1708885433</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181641423/prodam-skoda-octavia-20-tdi.php</t>
+  </si>
+  <si>
+    <t>Škoda octavia 2 combi</t>
+  </si>
+  <si>
+    <t>Jablonec nad Nisou 468 22</t>
+  </si>
+  <si>
+    <t>Prodám Škoda octavia 2 combi 2.0 tdi 103 kW Najeto 420 xxx km Nová STK Tažné zařízení, 3 RZ na tažné zařízení 6 stupňová manuální převodovka Spotřeba 5 - 6 l / 100km Dvouzónova klimatizace, Tempomat, Vyhřívaná zrcátka v el. K autu sada koberců gumové i textilní plus vana do kufru, ofuky ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/055/181595055.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181595055/skoda-octavia-2-combi.php</t>
+  </si>
+  <si>
+    <t>8.2. 2024</t>
+  </si>
+  <si>
+    <t>Náchod 547 01</t>
+  </si>
+  <si>
+    <t>Dobrý den, Prodám osobní automobil značky Škoda octavia II, facelift. R.V. 2010 Motor: 2.0tdi, 103kw, pohon 4x4 Manuální 6st převodovka STK platná do 3/2025 (v případě zájmu není problém při prodeji udělat novou STK) Výbava: Výhřev předních sedadel Zadní parkovací senzory Maxidot displ ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/716/181025716.jpg?t=1708937846</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181025716/skoda-octavia-2.php</t>
+  </si>
+  <si>
+    <t>Skoda Oktavia II 2.0.TDI 103kW</t>
+  </si>
+  <si>
+    <t>5.2. 2024</t>
+  </si>
+  <si>
+    <t>Praha - východ 250 70</t>
+  </si>
+  <si>
+    <t>Prodam Skoda octavia 2, 2.0 tdi 103kW, rv 2010, najezd 660000km, delane rozvody pri 600000km, plne pojizdne a funkcni, zimni+letni pneu Výbava vozu Bezpečnostní systémy: ABS, ESP Asistenční systémy: Parkovací senzory, Tempomat Zabezpečení vozidla: Alarm, Centrální zamykání, Dálkové cent ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/415/180253415.jpg?t=1706046589</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/180253415/skoda-oktavia-ii-20tdi-103kw.php</t>
+  </si>
+  <si>
+    <t>Škoda Octavia 2 vRS 2.0 TDI</t>
+  </si>
+  <si>
+    <t>České Budějovice 370 01</t>
+  </si>
+  <si>
+    <t>Rád bych prodal svoji Octavii 2 VRs, diesel 125kw (před fl upravenou na fl), kterou jsem v poslední době používal jako rezervní vozidlo, jelikož mám nový vůz v kombinaci se služebním, ale už pro ní nemám využití (celou dobu stojí v kryté garáži a občas jsem ji protáhl, aby nestála). Auto má najeto p ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/620/180179620.jpg?t=1708680487</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/180179620/skoda-octavia-2-vrs-20-tdi.php</t>
+  </si>
+  <si>
+    <t>Fabie 1,4 MPI ČR</t>
+  </si>
+  <si>
+    <t>Kolín 280 01</t>
+  </si>
+  <si>
+    <t>Škoda fabia 1.4 mpi. ČR R.V. 10/2000 202450 Servisní kniha Koupené v ČR Airbag Dálniční známka do září. Centrální zamykání na do Rádio s MP3 a USB Sada zimních Sada letních kol. Aktuálně po servisu oleje filtru brzd Čerstve po Stk. Stk. 2/26 Krásné tiché auticko ,bez dalších inv ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/173/181873173.jpg?t=1708955618</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181873173/fabie-14-mpi-cr.php</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181917682/koupim-skoda-fabia-i-ii-10-mpi-12-mpi-nebo-14-mpi.php</t>
+  </si>
+  <si>
+    <t>Škoda Fabia 1.4 MPi</t>
+  </si>
+  <si>
+    <t>Opava 747 05</t>
+  </si>
+  <si>
+    <t>Prodám Škoda fabia 1.4 mpi 44kw , rok výroby 2001 , najeto 185xxx Km , STK plátna do 1/2025 . Výbava : centrální zamykání, elektrické ovládání předních oken, posilovač řízení, nastavitelný volant, palubní počítač, výškově nastavitelná sedačka řidiče, odnímatelné tažné zařízení. Nyní děláno : hla ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/376/181887376.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181887376/skoda-fabia-14-mpi.php</t>
+  </si>
+  <si>
+    <t>Škoda Fabia combi 1.4MPi 50kw 2002/plně funkční</t>
+  </si>
+  <si>
+    <t>Prodám Škoda fabia kombi 1.4mpi 50kw, najeto 269000km, STK a Emise 8/2024, výbava: posilovač řízení, centrální zamykání, autorádio, Airbagy, 2xoriginál klíč, zámek zpátečky proti krádeži, plně funkční, minimum koroze, prahy zdravé, cena pevná, POUZE VOLAT DĚKUJI!!!</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/552/181884552.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181884552/skoda-fabia-combi-14mpi-50kw-2002plne-funkcni.php</t>
+  </si>
+  <si>
+    <t>ŠKODA FABIA I 1.4i MPI (2002) KOMBI</t>
+  </si>
+  <si>
+    <t>PRODÁM ) ŠKODA fabia I KOMBI, 1.4 mpi Benzín [50KW] R.V 2002) STK platná do 11/2025 ! ) nájezd: 230xxxtisíc) na autě vše pořádku stačí pouze sednout a jet v případě zájmu volejte nerezervuji ! kdo dřív příjde ten bere.</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/485/181867485.jpg</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181867485/skoda-fabia-i-14i-mpi-2002-kombi.php</t>
+  </si>
+  <si>
+    <t>Škoda fabia 1.4 MPI</t>
+  </si>
+  <si>
+    <t>Prodam Škoda fabia 1.4 mpi 50kw, stk do 8/2025,rok výroby 2000, najeto poctivých 148 000km ( možno prověřit přes cebia), auto vlastním 3 roky , jsem 1. Majitel v ČR , v Německu byl jeden majitel Klimatizace funkční , vyměněny čepy + stabilizační tycky, olej každý rok pravidelně , tažné zařízení , ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/295/181422295.jpg?t=1708699167</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/181422295/skoda-fabia-14-mpi.php</t>
+  </si>
+  <si>
+    <t>Škoda Fabia 1 1.4mpi</t>
+  </si>
+  <si>
+    <t>Prodám Fabii 14 mpi cena je pevná a vlastně cena je pouze za investice během dvou měsíců co jsem ji měl. Nové svíčky, nové rozvody, couvací senzory, nový výfuk, autu jsou úplně nové přední tlumiče značky Monro které jsou složené nové tlumiče nové pružiny nové uložení nové prachovky. Olej má najeto 5 ...</t>
+  </si>
+  <si>
+    <t>https://www.bazos.cz/img/1t/276/180790276.jpg?t=1707912883</t>
+  </si>
+  <si>
+    <t>https://auto.bazos.cz/inzerat/180790276/fabia-14mpi.php</t>
   </si>
 </sst>
 </file>
@@ -3536,7 +4031,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4AC74AD-538C-4782-8A8D-C4C0C7DD934D}">
-  <dimension ref="A1:N198"/>
+  <dimension ref="A1:N239"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D49" sqref="D49"/>
@@ -10859,6 +11354,1702 @@
         <v>1035</v>
       </c>
     </row>
+    <row r="199">
+      <c r="A199" t="s">
+        <v>466</v>
+      </c>
+      <c r="B199" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C199" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D199" t="s">
+        <v>390</v>
+      </c>
+      <c r="E199" t="s">
+        <v>1036</v>
+      </c>
+      <c r="F199" t="n">
+        <v>54000.0</v>
+      </c>
+      <c r="G199" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H199" t="s">
+        <v>393</v>
+      </c>
+      <c r="I199" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J199" t="s">
+        <v>1038</v>
+      </c>
+      <c r="K199" t="s">
+        <v>1039</v>
+      </c>
+      <c r="L199" t="s">
+        <v>1040</v>
+      </c>
+      <c r="M199" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="s">
+        <v>466</v>
+      </c>
+      <c r="B200" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C200" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D200" t="s">
+        <v>390</v>
+      </c>
+      <c r="E200" t="s">
+        <v>1042</v>
+      </c>
+      <c r="F200" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="G200" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H200" t="s">
+        <v>393</v>
+      </c>
+      <c r="I200" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J200" t="s">
+        <v>1043</v>
+      </c>
+      <c r="K200" t="s">
+        <v>1044</v>
+      </c>
+      <c r="L200" t="s">
+        <v>1045</v>
+      </c>
+      <c r="M200" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="s">
+        <v>466</v>
+      </c>
+      <c r="B201" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C201" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D201" t="s">
+        <v>390</v>
+      </c>
+      <c r="E201" t="s">
+        <v>467</v>
+      </c>
+      <c r="F201" t="n">
+        <v>68000.0</v>
+      </c>
+      <c r="G201" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H201" t="s">
+        <v>1047</v>
+      </c>
+      <c r="I201" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J201" t="s">
+        <v>468</v>
+      </c>
+      <c r="K201" t="s">
+        <v>1048</v>
+      </c>
+      <c r="L201" t="s">
+        <v>1049</v>
+      </c>
+      <c r="M201" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="s">
+        <v>466</v>
+      </c>
+      <c r="B202" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C202" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D202" t="s">
+        <v>390</v>
+      </c>
+      <c r="E202" t="s">
+        <v>1051</v>
+      </c>
+      <c r="F202" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="G202" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="H202" t="s">
+        <v>1052</v>
+      </c>
+      <c r="I202" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J202" t="s">
+        <v>253</v>
+      </c>
+      <c r="K202" t="s">
+        <v>1053</v>
+      </c>
+      <c r="L202" t="s">
+        <v>1054</v>
+      </c>
+      <c r="M202" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="s">
+        <v>466</v>
+      </c>
+      <c r="B203" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C203" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D203" t="s">
+        <v>390</v>
+      </c>
+      <c r="E203" t="s">
+        <v>1056</v>
+      </c>
+      <c r="F203" t="n">
+        <v>56000.0</v>
+      </c>
+      <c r="G203" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H203" t="s">
+        <v>1057</v>
+      </c>
+      <c r="I203" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J203" t="s">
+        <v>1058</v>
+      </c>
+      <c r="K203" t="s">
+        <v>1059</v>
+      </c>
+      <c r="L203" t="s">
+        <v>1060</v>
+      </c>
+      <c r="M203" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="s">
+        <v>421</v>
+      </c>
+      <c r="B204" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C204" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D204" t="s">
+        <v>390</v>
+      </c>
+      <c r="E204" t="s">
+        <v>1062</v>
+      </c>
+      <c r="F204" t="n">
+        <v>75000.0</v>
+      </c>
+      <c r="G204" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="H204" t="s">
+        <v>669</v>
+      </c>
+      <c r="I204" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J204" t="s">
+        <v>1063</v>
+      </c>
+      <c r="K204" t="s">
+        <v>1064</v>
+      </c>
+      <c r="L204" t="s">
+        <v>1065</v>
+      </c>
+      <c r="M204" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="s">
+        <v>466</v>
+      </c>
+      <c r="B205" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="C205" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D205" t="s">
+        <v>390</v>
+      </c>
+      <c r="E205" t="s">
+        <v>1036</v>
+      </c>
+      <c r="F205" t="n">
+        <v>54000.0</v>
+      </c>
+      <c r="G205" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="H205" t="s">
+        <v>579</v>
+      </c>
+      <c r="I205" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J205" t="s">
+        <v>1038</v>
+      </c>
+      <c r="K205" t="s">
+        <v>1039</v>
+      </c>
+      <c r="L205" t="s">
+        <v>1040</v>
+      </c>
+      <c r="M205" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s">
+        <v>466</v>
+      </c>
+      <c r="B206" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="C206" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D206" t="s">
+        <v>390</v>
+      </c>
+      <c r="E206" t="s">
+        <v>1042</v>
+      </c>
+      <c r="F206" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="G206" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="H206" t="s">
+        <v>430</v>
+      </c>
+      <c r="I206" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J206" t="s">
+        <v>1043</v>
+      </c>
+      <c r="K206" t="s">
+        <v>1044</v>
+      </c>
+      <c r="L206" t="s">
+        <v>1045</v>
+      </c>
+      <c r="M206" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s">
+        <v>466</v>
+      </c>
+      <c r="B207" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="C207" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D207" t="s">
+        <v>390</v>
+      </c>
+      <c r="E207" t="s">
+        <v>467</v>
+      </c>
+      <c r="F207" t="n">
+        <v>68000.0</v>
+      </c>
+      <c r="G207" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H207" t="s">
+        <v>1047</v>
+      </c>
+      <c r="I207" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J207" t="s">
+        <v>468</v>
+      </c>
+      <c r="K207" t="s">
+        <v>1048</v>
+      </c>
+      <c r="L207" t="s">
+        <v>1049</v>
+      </c>
+      <c r="M207" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="s">
+        <v>466</v>
+      </c>
+      <c r="B208" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="C208" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D208" t="s">
+        <v>390</v>
+      </c>
+      <c r="E208" t="s">
+        <v>1056</v>
+      </c>
+      <c r="F208" t="n">
+        <v>56000.0</v>
+      </c>
+      <c r="G208" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H208" t="s">
+        <v>1057</v>
+      </c>
+      <c r="I208" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J208" t="s">
+        <v>1058</v>
+      </c>
+      <c r="K208" t="s">
+        <v>1059</v>
+      </c>
+      <c r="L208" t="s">
+        <v>1060</v>
+      </c>
+      <c r="M208" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s">
+        <v>513</v>
+      </c>
+      <c r="B209" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C209" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D209" t="s">
+        <v>514</v>
+      </c>
+      <c r="E209" t="s">
+        <v>1067</v>
+      </c>
+      <c r="F209" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="G209" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H209" t="s">
+        <v>393</v>
+      </c>
+      <c r="I209" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J209" t="s">
+        <v>929</v>
+      </c>
+      <c r="K209" t="s">
+        <v>1068</v>
+      </c>
+      <c r="L209" t="s">
+        <v>1069</v>
+      </c>
+      <c r="M209" t="s">
+        <v>1070</v>
+      </c>
+      <c r="N209" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s">
+        <v>513</v>
+      </c>
+      <c r="B210" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C210" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D210" t="s">
+        <v>514</v>
+      </c>
+      <c r="E210" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F210" t="n">
+        <v>45000.0</v>
+      </c>
+      <c r="G210" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="H210" t="s">
+        <v>1052</v>
+      </c>
+      <c r="I210" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J210" t="s">
+        <v>1072</v>
+      </c>
+      <c r="K210" t="s">
+        <v>1073</v>
+      </c>
+      <c r="L210" t="s">
+        <v>1074</v>
+      </c>
+      <c r="M210" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s">
+        <v>521</v>
+      </c>
+      <c r="B211" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C211" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D211" t="s">
+        <v>514</v>
+      </c>
+      <c r="E211" t="s">
+        <v>271</v>
+      </c>
+      <c r="F211" t="n">
+        <v>54900.0</v>
+      </c>
+      <c r="G211" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H211" t="s">
+        <v>393</v>
+      </c>
+      <c r="I211" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J211" t="s">
+        <v>114</v>
+      </c>
+      <c r="K211" t="s">
+        <v>273</v>
+      </c>
+      <c r="L211" t="s">
+        <v>1076</v>
+      </c>
+      <c r="M211" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="s">
+        <v>521</v>
+      </c>
+      <c r="B212" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C212" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D212" t="s">
+        <v>514</v>
+      </c>
+      <c r="E212" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F212" t="n">
+        <v>55800.0</v>
+      </c>
+      <c r="G212" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H212" t="s">
+        <v>393</v>
+      </c>
+      <c r="I212" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J212" t="s">
+        <v>536</v>
+      </c>
+      <c r="K212" t="s">
+        <v>1079</v>
+      </c>
+      <c r="L212" t="s">
+        <v>1080</v>
+      </c>
+      <c r="M212" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s">
+        <v>521</v>
+      </c>
+      <c r="B213" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C213" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D213" t="s">
+        <v>514</v>
+      </c>
+      <c r="E213" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F213" t="n">
+        <v>85000.0</v>
+      </c>
+      <c r="G213" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="H213" t="s">
+        <v>1083</v>
+      </c>
+      <c r="I213" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J213" t="s">
+        <v>201</v>
+      </c>
+      <c r="K213" t="s">
+        <v>1084</v>
+      </c>
+      <c r="L213" t="s">
+        <v>1085</v>
+      </c>
+      <c r="M213" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="s">
+        <v>639</v>
+      </c>
+      <c r="B214" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C214" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D214" t="s">
+        <v>191</v>
+      </c>
+      <c r="E214" t="s">
+        <v>664</v>
+      </c>
+      <c r="F214" t="n">
+        <v>66000.0</v>
+      </c>
+      <c r="G214" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H214" t="s">
+        <v>1057</v>
+      </c>
+      <c r="I214" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J214" t="s">
+        <v>1087</v>
+      </c>
+      <c r="K214" t="s">
+        <v>647</v>
+      </c>
+      <c r="L214" t="s">
+        <v>1088</v>
+      </c>
+      <c r="M214" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="s">
+        <v>639</v>
+      </c>
+      <c r="B215" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C215" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D215" t="s">
+        <v>191</v>
+      </c>
+      <c r="E215" t="s">
+        <v>645</v>
+      </c>
+      <c r="F215" t="n">
+        <v>66000.0</v>
+      </c>
+      <c r="G215" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="H215" t="s">
+        <v>1052</v>
+      </c>
+      <c r="I215" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J215" t="s">
+        <v>1087</v>
+      </c>
+      <c r="K215" t="s">
+        <v>647</v>
+      </c>
+      <c r="L215" t="s">
+        <v>1090</v>
+      </c>
+      <c r="M215" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="s">
+        <v>639</v>
+      </c>
+      <c r="B216" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C216" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D216" t="s">
+        <v>191</v>
+      </c>
+      <c r="E216" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F216" t="n">
+        <v>45000.0</v>
+      </c>
+      <c r="G216" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="H216" t="s">
+        <v>392</v>
+      </c>
+      <c r="I216" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J216" t="s">
+        <v>1093</v>
+      </c>
+      <c r="K216" t="s">
+        <v>1094</v>
+      </c>
+      <c r="L216" t="s">
+        <v>1095</v>
+      </c>
+      <c r="M216" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="s">
+        <v>639</v>
+      </c>
+      <c r="B217" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C217" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D217" t="s">
+        <v>191</v>
+      </c>
+      <c r="E217" t="s">
+        <v>1097</v>
+      </c>
+      <c r="F217" t="n">
+        <v>90000.0</v>
+      </c>
+      <c r="G217" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H217" t="s">
+        <v>473</v>
+      </c>
+      <c r="I217" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J217" t="s">
+        <v>1098</v>
+      </c>
+      <c r="K217" t="s">
+        <v>1099</v>
+      </c>
+      <c r="L217" t="s">
+        <v>1100</v>
+      </c>
+      <c r="M217" t="s">
+        <v>1101</v>
+      </c>
+      <c r="N217" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="s">
+        <v>716</v>
+      </c>
+      <c r="B218" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C218" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D218" t="s">
+        <v>191</v>
+      </c>
+      <c r="E218" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F218" t="n">
+        <v>46900.0</v>
+      </c>
+      <c r="G218" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H218" t="s">
+        <v>393</v>
+      </c>
+      <c r="I218" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J218" t="s">
+        <v>317</v>
+      </c>
+      <c r="K218" t="s">
+        <v>1103</v>
+      </c>
+      <c r="L218" t="s">
+        <v>1104</v>
+      </c>
+      <c r="M218" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="s">
+        <v>716</v>
+      </c>
+      <c r="B219" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C219" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D219" t="s">
+        <v>191</v>
+      </c>
+      <c r="E219" t="s">
+        <v>1106</v>
+      </c>
+      <c r="F219" t="n">
+        <v>55000.0</v>
+      </c>
+      <c r="G219" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H219" t="s">
+        <v>393</v>
+      </c>
+      <c r="I219" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J219" t="s">
+        <v>760</v>
+      </c>
+      <c r="K219" t="s">
+        <v>1107</v>
+      </c>
+      <c r="L219" t="s">
+        <v>1108</v>
+      </c>
+      <c r="M219" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="s">
+        <v>716</v>
+      </c>
+      <c r="B220" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C220" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D220" t="s">
+        <v>191</v>
+      </c>
+      <c r="E220" t="s">
+        <v>1110</v>
+      </c>
+      <c r="F220" t="n">
+        <v>55000.0</v>
+      </c>
+      <c r="G220" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H220" t="s">
+        <v>393</v>
+      </c>
+      <c r="I220" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J220" t="s">
+        <v>1111</v>
+      </c>
+      <c r="K220" t="s">
+        <v>1112</v>
+      </c>
+      <c r="L220" t="s">
+        <v>1113</v>
+      </c>
+      <c r="M220" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="s">
+        <v>716</v>
+      </c>
+      <c r="B221" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C221" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D221" t="s">
+        <v>191</v>
+      </c>
+      <c r="E221" t="s">
+        <v>1115</v>
+      </c>
+      <c r="F221" t="n">
+        <v>56000.0</v>
+      </c>
+      <c r="G221" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H221" t="s">
+        <v>1047</v>
+      </c>
+      <c r="I221" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J221" t="s">
+        <v>206</v>
+      </c>
+      <c r="K221" t="s">
+        <v>1116</v>
+      </c>
+      <c r="L221" t="s">
+        <v>1117</v>
+      </c>
+      <c r="M221" t="s">
+        <v>1118</v>
+      </c>
+      <c r="N221" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="s">
+        <v>716</v>
+      </c>
+      <c r="B222" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C222" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D222" t="s">
+        <v>191</v>
+      </c>
+      <c r="E222" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F222" t="n">
+        <v>79000.0</v>
+      </c>
+      <c r="G222" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H222" t="s">
+        <v>1057</v>
+      </c>
+      <c r="I222" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J222" t="s">
+        <v>1120</v>
+      </c>
+      <c r="K222" t="s">
+        <v>1121</v>
+      </c>
+      <c r="L222" t="s">
+        <v>1122</v>
+      </c>
+      <c r="M222" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="s">
+        <v>716</v>
+      </c>
+      <c r="B223" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C223" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D223" t="s">
+        <v>191</v>
+      </c>
+      <c r="E223" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F223" t="n">
+        <v>65000.0</v>
+      </c>
+      <c r="G223" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="H223" t="s">
+        <v>441</v>
+      </c>
+      <c r="I223" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J223" t="s">
+        <v>1125</v>
+      </c>
+      <c r="K223" t="s">
+        <v>1126</v>
+      </c>
+      <c r="L223" t="s">
+        <v>1127</v>
+      </c>
+      <c r="M223" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="s">
+        <v>716</v>
+      </c>
+      <c r="B224" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C224" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D224" t="s">
+        <v>191</v>
+      </c>
+      <c r="E224" t="s">
+        <v>1129</v>
+      </c>
+      <c r="F224" t="n">
+        <v>49999.0</v>
+      </c>
+      <c r="G224" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H224" t="s">
+        <v>473</v>
+      </c>
+      <c r="I224" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J224" t="s">
+        <v>1130</v>
+      </c>
+      <c r="K224" t="s">
+        <v>1131</v>
+      </c>
+      <c r="L224" t="s">
+        <v>1132</v>
+      </c>
+      <c r="M224" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="s">
+        <v>716</v>
+      </c>
+      <c r="B225" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C225" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D225" t="s">
+        <v>191</v>
+      </c>
+      <c r="E225" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F225" t="n">
+        <v>48000.0</v>
+      </c>
+      <c r="G225" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="H225" t="s">
+        <v>398</v>
+      </c>
+      <c r="I225" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J225" t="s">
+        <v>1135</v>
+      </c>
+      <c r="K225" t="s">
+        <v>1136</v>
+      </c>
+      <c r="L225" t="s">
+        <v>1137</v>
+      </c>
+      <c r="M225" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="s">
+        <v>829</v>
+      </c>
+      <c r="B226" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C226" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D226" t="s">
+        <v>191</v>
+      </c>
+      <c r="E226" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F226" t="n">
+        <v>88000.0</v>
+      </c>
+      <c r="G226" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="H226" t="s">
+        <v>430</v>
+      </c>
+      <c r="I226" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J226" t="s">
+        <v>1140</v>
+      </c>
+      <c r="K226" t="s">
+        <v>1141</v>
+      </c>
+      <c r="L226" t="s">
+        <v>1142</v>
+      </c>
+      <c r="M226" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="s">
+        <v>829</v>
+      </c>
+      <c r="B227" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C227" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D227" t="s">
+        <v>191</v>
+      </c>
+      <c r="E227" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F227" t="n">
+        <v>79000.0</v>
+      </c>
+      <c r="G227" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="H227" t="s">
+        <v>1052</v>
+      </c>
+      <c r="I227" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J227" t="s">
+        <v>1145</v>
+      </c>
+      <c r="K227" t="s">
+        <v>1146</v>
+      </c>
+      <c r="L227" t="s">
+        <v>1147</v>
+      </c>
+      <c r="M227" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="s">
+        <v>829</v>
+      </c>
+      <c r="B228" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C228" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D228" t="s">
+        <v>191</v>
+      </c>
+      <c r="E228" t="s">
+        <v>1149</v>
+      </c>
+      <c r="F228" t="n">
+        <v>68000.0</v>
+      </c>
+      <c r="G228" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="H228" t="s">
+        <v>516</v>
+      </c>
+      <c r="I228" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J228" t="s">
+        <v>290</v>
+      </c>
+      <c r="K228" t="s">
+        <v>1150</v>
+      </c>
+      <c r="L228" t="s">
+        <v>1151</v>
+      </c>
+      <c r="M228" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="s">
+        <v>829</v>
+      </c>
+      <c r="B229" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C229" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D229" t="s">
+        <v>191</v>
+      </c>
+      <c r="E229" t="s">
+        <v>1153</v>
+      </c>
+      <c r="F229" t="n">
+        <v>52000.0</v>
+      </c>
+      <c r="G229" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="H229" t="s">
+        <v>430</v>
+      </c>
+      <c r="I229" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J229" t="s">
+        <v>1154</v>
+      </c>
+      <c r="K229" t="s">
+        <v>1155</v>
+      </c>
+      <c r="L229" t="s">
+        <v>1156</v>
+      </c>
+      <c r="M229" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="s">
+        <v>829</v>
+      </c>
+      <c r="B230" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C230" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D230" t="s">
+        <v>191</v>
+      </c>
+      <c r="E230" t="s">
+        <v>650</v>
+      </c>
+      <c r="F230" t="n">
+        <v>85000.0</v>
+      </c>
+      <c r="G230" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="H230" t="s">
+        <v>1158</v>
+      </c>
+      <c r="I230" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J230" t="s">
+        <v>1159</v>
+      </c>
+      <c r="K230" t="s">
+        <v>1160</v>
+      </c>
+      <c r="L230" t="s">
+        <v>1161</v>
+      </c>
+      <c r="M230" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="s">
+        <v>829</v>
+      </c>
+      <c r="B231" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C231" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D231" t="s">
+        <v>191</v>
+      </c>
+      <c r="E231" t="s">
+        <v>1163</v>
+      </c>
+      <c r="F231" t="n">
+        <v>68000.0</v>
+      </c>
+      <c r="G231" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="H231" t="s">
+        <v>1164</v>
+      </c>
+      <c r="I231" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J231" t="s">
+        <v>1165</v>
+      </c>
+      <c r="K231" t="s">
+        <v>1166</v>
+      </c>
+      <c r="L231" t="s">
+        <v>1167</v>
+      </c>
+      <c r="M231" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="s">
+        <v>829</v>
+      </c>
+      <c r="B232" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="C232" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="D232" t="s">
+        <v>191</v>
+      </c>
+      <c r="E232" t="s">
+        <v>1169</v>
+      </c>
+      <c r="F232" t="n">
+        <v>70000.0</v>
+      </c>
+      <c r="G232" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="H232" t="s">
+        <v>798</v>
+      </c>
+      <c r="I232" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J232" t="s">
+        <v>1170</v>
+      </c>
+      <c r="K232" t="s">
+        <v>1171</v>
+      </c>
+      <c r="L232" t="s">
+        <v>1172</v>
+      </c>
+      <c r="M232" t="s">
+        <v>1173</v>
+      </c>
+      <c r="N232" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="s">
+        <v>938</v>
+      </c>
+      <c r="B233" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="C233" t="n">
+        <v>35000.0</v>
+      </c>
+      <c r="D233" t="s">
+        <v>939</v>
+      </c>
+      <c r="E233" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F233" t="n">
+        <v>27000.0</v>
+      </c>
+      <c r="G233" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H233" t="s">
+        <v>393</v>
+      </c>
+      <c r="I233" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J233" t="s">
+        <v>1175</v>
+      </c>
+      <c r="K233" t="s">
+        <v>1176</v>
+      </c>
+      <c r="L233" t="s">
+        <v>1177</v>
+      </c>
+      <c r="M233" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="s">
+        <v>938</v>
+      </c>
+      <c r="B234" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="C234" t="n">
+        <v>35000.0</v>
+      </c>
+      <c r="D234" t="s">
+        <v>939</v>
+      </c>
+      <c r="E234" t="s">
+        <v>333</v>
+      </c>
+      <c r="F234" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="G234" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H234" t="s">
+        <v>393</v>
+      </c>
+      <c r="I234" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J234" t="s">
+        <v>335</v>
+      </c>
+      <c r="K234" t="s">
+        <v>336</v>
+      </c>
+      <c r="L234" t="s">
+        <v>337</v>
+      </c>
+      <c r="M234" t="s">
+        <v>1179</v>
+      </c>
+      <c r="N234" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="s">
+        <v>938</v>
+      </c>
+      <c r="B235" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="C235" t="n">
+        <v>35000.0</v>
+      </c>
+      <c r="D235" t="s">
+        <v>939</v>
+      </c>
+      <c r="E235" t="s">
+        <v>1180</v>
+      </c>
+      <c r="F235" t="n">
+        <v>35000.0</v>
+      </c>
+      <c r="G235" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H235" t="s">
+        <v>1047</v>
+      </c>
+      <c r="I235" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J235" t="s">
+        <v>1181</v>
+      </c>
+      <c r="K235" t="s">
+        <v>1182</v>
+      </c>
+      <c r="L235" t="s">
+        <v>1183</v>
+      </c>
+      <c r="M235" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="s">
+        <v>938</v>
+      </c>
+      <c r="B236" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="C236" t="n">
+        <v>35000.0</v>
+      </c>
+      <c r="D236" t="s">
+        <v>939</v>
+      </c>
+      <c r="E236" t="s">
+        <v>1185</v>
+      </c>
+      <c r="F236" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="G236" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H236" t="s">
+        <v>1047</v>
+      </c>
+      <c r="I236" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J236" t="s">
+        <v>335</v>
+      </c>
+      <c r="K236" t="s">
+        <v>1186</v>
+      </c>
+      <c r="L236" t="s">
+        <v>1187</v>
+      </c>
+      <c r="M236" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="s">
+        <v>938</v>
+      </c>
+      <c r="B237" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="C237" t="n">
+        <v>35000.0</v>
+      </c>
+      <c r="D237" t="s">
+        <v>939</v>
+      </c>
+      <c r="E237" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F237" t="n">
+        <v>25000.0</v>
+      </c>
+      <c r="G237" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H237" t="s">
+        <v>1047</v>
+      </c>
+      <c r="I237" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J237" t="s">
+        <v>399</v>
+      </c>
+      <c r="K237" t="s">
+        <v>1190</v>
+      </c>
+      <c r="L237" t="s">
+        <v>1191</v>
+      </c>
+      <c r="M237" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="s">
+        <v>938</v>
+      </c>
+      <c r="B238" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="C238" t="n">
+        <v>35000.0</v>
+      </c>
+      <c r="D238" t="s">
+        <v>939</v>
+      </c>
+      <c r="E238" t="s">
+        <v>1193</v>
+      </c>
+      <c r="F238" t="n">
+        <v>26990.0</v>
+      </c>
+      <c r="G238" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="H238" t="s">
+        <v>441</v>
+      </c>
+      <c r="I238" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J238" t="s">
+        <v>570</v>
+      </c>
+      <c r="K238" t="s">
+        <v>1194</v>
+      </c>
+      <c r="L238" t="s">
+        <v>1195</v>
+      </c>
+      <c r="M238" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="s">
+        <v>938</v>
+      </c>
+      <c r="B239" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="C239" t="n">
+        <v>35000.0</v>
+      </c>
+      <c r="D239" t="s">
+        <v>939</v>
+      </c>
+      <c r="E239" t="s">
+        <v>1197</v>
+      </c>
+      <c r="F239" t="n">
+        <v>33000.0</v>
+      </c>
+      <c r="G239" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="H239" t="s">
+        <v>793</v>
+      </c>
+      <c r="I239" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J239" t="s">
+        <v>746</v>
+      </c>
+      <c r="K239" t="s">
+        <v>1198</v>
+      </c>
+      <c r="L239" t="s">
+        <v>1199</v>
+      </c>
+      <c r="M239" t="s">
+        <v>1200</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I54" r:id="rId1" xr:uid="{6B848895-FAD7-4421-AB5E-A9D0B4A79CEF}"/>

</xml_diff>